<commit_message>
Subject data is updated(Excel file)
</commit_message>
<xml_diff>
--- a/smartglove_data_form.xlsx
+++ b/smartglove_data_form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kanghae Choi\Dropbox\2_Hanyang\2_기술경영전문대학원 석사\1_석사 연구\1_스마트글러브\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kanghae Choi\Dropbox\3_program_code\GITHUB\imaginexlab_smartglove\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EDA533-168E-492A-8685-248913B9E2A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36BAE08-4BE8-4973-8086-16D696F496B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="478" xr2:uid="{DEA0BA13-803F-4C08-A035-B07F2889F4B2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -218,6 +218,24 @@
   </si>
   <si>
     <t>민</t>
+  </si>
+  <si>
+    <t>Numer of M</t>
+  </si>
+  <si>
+    <t>Number of F</t>
+  </si>
+  <si>
+    <t>Ratio F/M</t>
+  </si>
+  <si>
+    <t>민정</t>
+  </si>
+  <si>
+    <t>은아</t>
+  </si>
+  <si>
+    <t>신희</t>
   </si>
 </sst>
 </file>
@@ -589,30 +607,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -635,6 +629,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -964,8 +982,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -984,17 +1002,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="37"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="29"/>
       <c r="J1" t="s">
         <v>17</v>
       </c>
@@ -1003,15 +1021,15 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A2" s="38"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="40"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32"/>
       <c r="J2" t="s">
         <v>18</v>
       </c>
@@ -1101,12 +1119,12 @@
         <v>29</v>
       </c>
       <c r="O4" s="2"/>
-      <c r="P4" s="41" t="s">
+      <c r="P4" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="42"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="34"/>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="6" t="s">
@@ -1147,12 +1165,12 @@
         <v>8</v>
       </c>
       <c r="O5" s="2"/>
-      <c r="P5" s="31" t="s">
+      <c r="P5" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="32"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="36"/>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="6" t="s">
@@ -1193,12 +1211,12 @@
         <v>2</v>
       </c>
       <c r="O6" s="2"/>
-      <c r="P6" s="31" t="s">
+      <c r="P6" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="32"/>
+      <c r="Q6" s="35"/>
+      <c r="R6" s="35"/>
+      <c r="S6" s="36"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="6" t="s">
@@ -1239,12 +1257,12 @@
         <v>9</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="31" t="s">
+      <c r="P7" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="32"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="36"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="6" t="s">
@@ -1281,16 +1299,16 @@
         <v>5</v>
       </c>
       <c r="K8" s="3"/>
-      <c r="N8" s="29" t="s">
+      <c r="N8" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="30"/>
-      <c r="P8" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="32"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="35"/>
+      <c r="S8" s="36"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="6" t="s">
@@ -1327,14 +1345,14 @@
         <v>6</v>
       </c>
       <c r="K9" s="3"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="31" t="s">
+      <c r="N9" s="39"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="32"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="36"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="6" t="s">
@@ -1375,12 +1393,12 @@
         <v>14</v>
       </c>
       <c r="O10" s="2"/>
-      <c r="P10" s="33">
+      <c r="P10" s="41">
         <v>4.5891203703703705E-2</v>
       </c>
-      <c r="Q10" s="33"/>
-      <c r="R10" s="33"/>
-      <c r="S10" s="34"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="42"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="6" t="s">
@@ -1421,12 +1439,12 @@
         <v>15</v>
       </c>
       <c r="O11" s="2"/>
-      <c r="P11" s="31" t="s">
+      <c r="P11" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="32"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="36"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1">
       <c r="A12" s="6" t="s">
@@ -1467,12 +1485,12 @@
         <v>16</v>
       </c>
       <c r="O12" s="19"/>
-      <c r="P12" s="27" t="s">
+      <c r="P12" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="28"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="38"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="6" t="s">
@@ -1617,8 +1635,15 @@
         <v>13</v>
       </c>
       <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="M16" t="s">
+        <v>60</v>
+      </c>
+      <c r="O16">
+        <f>SUMPRODUCT(LEN(D4:D63)-LEN(SUBSTITUTE(D4:D63,"M","")))</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="6" t="s">
         <v>42</v>
       </c>
@@ -1653,8 +1678,15 @@
         <v>14</v>
       </c>
       <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="M17" t="s">
+        <v>61</v>
+      </c>
+      <c r="O17">
+        <f>SUMPRODUCT(LEN(D4:D63)-LEN(SUBSTITUTE(D4:D63,"F","")))</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
@@ -1689,8 +1721,15 @@
         <v>15</v>
       </c>
       <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="M18" t="s">
+        <v>62</v>
+      </c>
+      <c r="O18">
+        <f>O17/O16</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="6" t="s">
         <v>44</v>
       </c>
@@ -1726,7 +1765,7 @@
       </c>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:15">
       <c r="A20" s="6" t="s">
         <v>44</v>
       </c>
@@ -1762,7 +1801,7 @@
       </c>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:15">
       <c r="A21" s="6" t="s">
         <v>44</v>
       </c>
@@ -1798,7 +1837,7 @@
       </c>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:15">
       <c r="A22" s="6" t="s">
         <v>46</v>
       </c>
@@ -1834,7 +1873,7 @@
       </c>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:15">
       <c r="A23" s="6" t="s">
         <v>46</v>
       </c>
@@ -1870,7 +1909,7 @@
       </c>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:15">
       <c r="A24" s="6" t="s">
         <v>46</v>
       </c>
@@ -1906,7 +1945,7 @@
       </c>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:15">
       <c r="A25" s="6" t="s">
         <v>48</v>
       </c>
@@ -1942,7 +1981,7 @@
       </c>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:15">
       <c r="A26" s="6" t="s">
         <v>48</v>
       </c>
@@ -1978,7 +2017,7 @@
       </c>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:15">
       <c r="A27" s="6" t="s">
         <v>48</v>
       </c>
@@ -2014,7 +2053,7 @@
       </c>
       <c r="K27" s="3"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:15">
       <c r="A28" s="6" t="s">
         <v>50</v>
       </c>
@@ -2050,7 +2089,7 @@
       </c>
       <c r="K28" s="3"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:15">
       <c r="A29" s="6" t="s">
         <v>50</v>
       </c>
@@ -2086,7 +2125,7 @@
       </c>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:15">
       <c r="A30" s="6" t="s">
         <v>50</v>
       </c>
@@ -2122,7 +2161,7 @@
       </c>
       <c r="K30" s="3"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:15">
       <c r="A31" s="6" t="s">
         <v>52</v>
       </c>
@@ -2158,7 +2197,7 @@
       </c>
       <c r="K31" s="3"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:15">
       <c r="A32" s="6" t="s">
         <v>52</v>
       </c>
@@ -2663,11 +2702,21 @@
       <c r="K45" s="3"/>
     </row>
     <row r="46" spans="1:11">
-      <c r="A46" s="6"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
+      <c r="A46" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="3">
+        <v>1993</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F46" s="3" t="s">
         <v>12</v>
       </c>
@@ -2689,11 +2738,21 @@
       <c r="K46" s="3"/>
     </row>
     <row r="47" spans="1:11">
-      <c r="A47" s="6"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
+      <c r="A47" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="3">
+        <v>1993</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F47" s="3" t="s">
         <v>12</v>
       </c>
@@ -2715,11 +2774,21 @@
       <c r="K47" s="3"/>
     </row>
     <row r="48" spans="1:11">
-      <c r="A48" s="6"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
+      <c r="A48" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" s="3">
+        <v>1993</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F48" s="3" t="s">
         <v>12</v>
       </c>
@@ -2741,11 +2810,21 @@
       <c r="K48" s="3"/>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="6"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
+      <c r="A49" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="3">
+        <v>1993</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F49" s="3" t="s">
         <v>12</v>
       </c>
@@ -2767,11 +2846,21 @@
       <c r="K49" s="3"/>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="6"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
+      <c r="A50" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" s="3">
+        <v>1993</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F50" s="3" t="s">
         <v>12</v>
       </c>
@@ -2793,11 +2882,21 @@
       <c r="K50" s="3"/>
     </row>
     <row r="51" spans="1:11">
-      <c r="A51" s="6"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
+      <c r="A51" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="3">
+        <v>1993</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F51" s="3" t="s">
         <v>12</v>
       </c>
@@ -2819,11 +2918,21 @@
       <c r="K51" s="3"/>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="6"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
+      <c r="A52" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" s="3">
+        <v>1995</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F52" s="3" t="s">
         <v>12</v>
       </c>
@@ -2845,11 +2954,21 @@
       <c r="K52" s="3"/>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="6"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
+      <c r="A53" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" s="3">
+        <v>1995</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F53" s="3" t="s">
         <v>12</v>
       </c>
@@ -2871,11 +2990,21 @@
       <c r="K53" s="3"/>
     </row>
     <row r="54" spans="1:11">
-      <c r="A54" s="6"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
+      <c r="A54" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" s="3">
+        <v>1995</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F54" s="3" t="s">
         <v>12</v>
       </c>
@@ -3004,7 +3133,7 @@
       <c r="A59" s="8"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
+      <c r="D59" s="3"/>
       <c r="E59" s="9"/>
       <c r="F59" s="9" t="s">
         <v>12</v>
@@ -3030,7 +3159,7 @@
       <c r="A60" s="8"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
+      <c r="D60" s="3"/>
       <c r="E60" s="9"/>
       <c r="F60" s="9" t="s">
         <v>12</v>
@@ -3510,17 +3639,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="P5:S5"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="P7:S7"/>
     <mergeCell ref="P12:S12"/>
     <mergeCell ref="N8:O9"/>
     <mergeCell ref="P8:S8"/>
     <mergeCell ref="P9:S9"/>
     <mergeCell ref="P10:S10"/>
     <mergeCell ref="P11:S11"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="P7:S7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3533,7 +3662,7 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3552,17 +3681,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="37"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="29"/>
       <c r="J1" t="s">
         <v>17</v>
       </c>
@@ -3636,12 +3765,12 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="str">
-        <f>CONCATENATE("Hand_IMU_20_",J3+1,".txt")</f>
-        <v>Hand_IMU_20_1.txt</v>
+        <f>CONCATENATE("Hand_IMU_60_",J3+1,".txt")</f>
+        <v>Hand_IMU_60_1.txt</v>
       </c>
       <c r="I4" s="7" t="str">
-        <f>CONCATENATE("Wrist_IMU_20_",J3+1,".txt")</f>
-        <v>Wrist_IMU_20_1.txt</v>
+        <f>CONCATENATE("Wrist_IMU_60_",J3+1,".txt")</f>
+        <v>Wrist_IMU_60_1.txt</v>
       </c>
       <c r="J4" s="14">
         <f>J3+1</f>
@@ -3654,12 +3783,12 @@
         <v>29</v>
       </c>
       <c r="O4" s="2"/>
-      <c r="P4" s="41" t="s">
+      <c r="P4" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="42"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="34"/>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="6"/>
@@ -3670,12 +3799,12 @@
       <c r="F5" s="3"/>
       <c r="G5" s="12"/>
       <c r="H5" s="3" t="str">
-        <f t="shared" ref="H5:H22" si="0">CONCATENATE("Hand_IMU_20_",J4+1,".txt")</f>
-        <v>Hand_IMU_20_2.txt</v>
+        <f t="shared" ref="H5:H22" si="0">CONCATENATE("Hand_IMU_60_",J4+1,".txt")</f>
+        <v>Hand_IMU_60_2.txt</v>
       </c>
       <c r="I5" s="7" t="str">
-        <f t="shared" ref="I5:I22" si="1">CONCATENATE("Wrist_IMU_20_",J4+1,".txt")</f>
-        <v>Wrist_IMU_20_2.txt</v>
+        <f t="shared" ref="I5:I22" si="1">CONCATENATE("Wrist_IMU_60_",J4+1,".txt")</f>
+        <v>Wrist_IMU_60_2.txt</v>
       </c>
       <c r="J5" s="14">
         <f t="shared" ref="J5:J22" si="2">J4+1</f>
@@ -3686,12 +3815,12 @@
         <v>8</v>
       </c>
       <c r="O5" s="2"/>
-      <c r="P5" s="31" t="s">
+      <c r="P5" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="32"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="36"/>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="6"/>
@@ -3703,11 +3832,11 @@
       <c r="G6" s="12"/>
       <c r="H6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Hand_IMU_20_3.txt</v>
+        <v>Hand_IMU_60_3.txt</v>
       </c>
       <c r="I6" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Wrist_IMU_20_3.txt</v>
+        <v>Wrist_IMU_60_3.txt</v>
       </c>
       <c r="J6" s="14">
         <f t="shared" si="2"/>
@@ -3718,12 +3847,12 @@
         <v>2</v>
       </c>
       <c r="O6" s="2"/>
-      <c r="P6" s="31" t="s">
+      <c r="P6" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="32"/>
+      <c r="Q6" s="35"/>
+      <c r="R6" s="35"/>
+      <c r="S6" s="36"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="6"/>
@@ -3734,12 +3863,12 @@
       <c r="F7" s="3"/>
       <c r="G7" s="12"/>
       <c r="H7" s="3" t="str">
-        <f>CONCATENATE("Hand_IMU_20_",J6+1,".txt")</f>
-        <v>Hand_IMU_20_4.txt</v>
+        <f t="shared" si="0"/>
+        <v>Hand_IMU_60_4.txt</v>
       </c>
       <c r="I7" s="7" t="str">
-        <f>CONCATENATE("Wrist_IMU_20_",J6+1,".txt")</f>
-        <v>Wrist_IMU_20_4.txt</v>
+        <f t="shared" si="1"/>
+        <v>Wrist_IMU_60_4.txt</v>
       </c>
       <c r="J7" s="14">
         <f>J6+1</f>
@@ -3750,12 +3879,12 @@
         <v>9</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="31" t="s">
+      <c r="P7" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="32"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="36"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="6"/>
@@ -3767,27 +3896,27 @@
       <c r="G8" s="12"/>
       <c r="H8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Hand_IMU_20_5.txt</v>
+        <v>Hand_IMU_60_5.txt</v>
       </c>
       <c r="I8" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Wrist_IMU_20_5.txt</v>
+        <v>Wrist_IMU_60_5.txt</v>
       </c>
       <c r="J8" s="14">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="K8" s="3"/>
-      <c r="N8" s="29" t="s">
+      <c r="N8" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="30"/>
-      <c r="P8" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="32"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="35"/>
+      <c r="S8" s="36"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="6"/>
@@ -3799,25 +3928,25 @@
       <c r="G9" s="12"/>
       <c r="H9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Hand_IMU_20_6.txt</v>
+        <v>Hand_IMU_60_6.txt</v>
       </c>
       <c r="I9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Wrist_IMU_20_6.txt</v>
+        <v>Wrist_IMU_60_6.txt</v>
       </c>
       <c r="J9" s="14">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="K9" s="3"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="31" t="s">
+      <c r="N9" s="39"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="32"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="36"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="6"/>
@@ -3829,11 +3958,11 @@
       <c r="G10" s="12"/>
       <c r="H10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Hand_IMU_20_7.txt</v>
+        <v>Hand_IMU_60_7.txt</v>
       </c>
       <c r="I10" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Wrist_IMU_20_7.txt</v>
+        <v>Wrist_IMU_60_7.txt</v>
       </c>
       <c r="J10" s="14">
         <f t="shared" si="2"/>
@@ -3844,12 +3973,12 @@
         <v>14</v>
       </c>
       <c r="O10" s="2"/>
-      <c r="P10" s="33">
+      <c r="P10" s="41">
         <v>4.5891203703703705E-2</v>
       </c>
-      <c r="Q10" s="33"/>
-      <c r="R10" s="33"/>
-      <c r="S10" s="34"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="42"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="6"/>
@@ -3861,11 +3990,11 @@
       <c r="G11" s="12"/>
       <c r="H11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Hand_IMU_20_8.txt</v>
+        <v>Hand_IMU_60_8.txt</v>
       </c>
       <c r="I11" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Wrist_IMU_20_8.txt</v>
+        <v>Wrist_IMU_60_8.txt</v>
       </c>
       <c r="J11" s="14">
         <f t="shared" si="2"/>
@@ -3876,12 +4005,12 @@
         <v>15</v>
       </c>
       <c r="O11" s="2"/>
-      <c r="P11" s="31" t="s">
+      <c r="P11" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="32"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="36"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1">
       <c r="A12" s="6"/>
@@ -3893,11 +4022,11 @@
       <c r="G12" s="12"/>
       <c r="H12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Hand_IMU_20_9.txt</v>
+        <v>Hand_IMU_60_9.txt</v>
       </c>
       <c r="I12" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Wrist_IMU_20_9.txt</v>
+        <v>Wrist_IMU_60_9.txt</v>
       </c>
       <c r="J12" s="14">
         <f t="shared" si="2"/>
@@ -3908,12 +4037,12 @@
         <v>16</v>
       </c>
       <c r="O12" s="19"/>
-      <c r="P12" s="27" t="s">
+      <c r="P12" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="28"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="38"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="6"/>
@@ -3925,11 +4054,11 @@
       <c r="G13" s="12"/>
       <c r="H13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Hand_IMU_20_10.txt</v>
+        <v>Hand_IMU_60_10.txt</v>
       </c>
       <c r="I13" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Wrist_IMU_20_10.txt</v>
+        <v>Wrist_IMU_60_10.txt</v>
       </c>
       <c r="J13" s="14">
         <f t="shared" si="2"/>
@@ -3947,11 +4076,11 @@
       <c r="G14" s="12"/>
       <c r="H14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Hand_IMU_20_11.txt</v>
+        <v>Hand_IMU_60_11.txt</v>
       </c>
       <c r="I14" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Wrist_IMU_20_11.txt</v>
+        <v>Wrist_IMU_60_11.txt</v>
       </c>
       <c r="J14" s="14">
         <f t="shared" si="2"/>
@@ -3969,11 +4098,11 @@
       <c r="G15" s="12"/>
       <c r="H15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Hand_IMU_20_12.txt</v>
+        <v>Hand_IMU_60_12.txt</v>
       </c>
       <c r="I15" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Wrist_IMU_20_12.txt</v>
+        <v>Wrist_IMU_60_12.txt</v>
       </c>
       <c r="J15" s="14">
         <f t="shared" si="2"/>
@@ -3991,11 +4120,11 @@
       <c r="G16" s="12"/>
       <c r="H16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Hand_IMU_20_13.txt</v>
+        <v>Hand_IMU_60_13.txt</v>
       </c>
       <c r="I16" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Wrist_IMU_20_13.txt</v>
+        <v>Wrist_IMU_60_13.txt</v>
       </c>
       <c r="J16" s="14">
         <f t="shared" si="2"/>
@@ -4013,11 +4142,11 @@
       <c r="G17" s="12"/>
       <c r="H17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Hand_IMU_20_14.txt</v>
+        <v>Hand_IMU_60_14.txt</v>
       </c>
       <c r="I17" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Wrist_IMU_20_14.txt</v>
+        <v>Wrist_IMU_60_14.txt</v>
       </c>
       <c r="J17" s="14">
         <f t="shared" si="2"/>
@@ -4035,11 +4164,11 @@
       <c r="G18" s="12"/>
       <c r="H18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Hand_IMU_20_15.txt</v>
+        <v>Hand_IMU_60_15.txt</v>
       </c>
       <c r="I18" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Wrist_IMU_20_15.txt</v>
+        <v>Wrist_IMU_60_15.txt</v>
       </c>
       <c r="J18" s="14">
         <f t="shared" si="2"/>
@@ -4057,11 +4186,11 @@
       <c r="G19" s="12"/>
       <c r="H19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Hand_IMU_20_16.txt</v>
+        <v>Hand_IMU_60_16.txt</v>
       </c>
       <c r="I19" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Wrist_IMU_20_16.txt</v>
+        <v>Wrist_IMU_60_16.txt</v>
       </c>
       <c r="J19" s="14">
         <f t="shared" si="2"/>
@@ -4079,11 +4208,11 @@
       <c r="G20" s="12"/>
       <c r="H20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Hand_IMU_20_17.txt</v>
+        <v>Hand_IMU_60_17.txt</v>
       </c>
       <c r="I20" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Wrist_IMU_20_17.txt</v>
+        <v>Wrist_IMU_60_17.txt</v>
       </c>
       <c r="J20" s="14">
         <f t="shared" si="2"/>
@@ -4101,11 +4230,11 @@
       <c r="G21" s="12"/>
       <c r="H21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Hand_IMU_20_18.txt</v>
+        <v>Hand_IMU_60_18.txt</v>
       </c>
       <c r="I21" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Wrist_IMU_20_18.txt</v>
+        <v>Wrist_IMU_60_18.txt</v>
       </c>
       <c r="J21" s="14">
         <f t="shared" si="2"/>
@@ -4121,13 +4250,13 @@
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="13"/>
-      <c r="H22" s="9" t="str">
+      <c r="H22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Hand_IMU_20_19.txt</v>
-      </c>
-      <c r="I22" s="10" t="str">
+        <v>Hand_IMU_60_19.txt</v>
+      </c>
+      <c r="I22" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>Wrist_IMU_20_19.txt</v>
+        <v>Wrist_IMU_60_19.txt</v>
       </c>
       <c r="J22" s="14">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Feature scaling function is added
</commit_message>
<xml_diff>
--- a/smartglove_data_form.xlsx
+++ b/smartglove_data_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kanghae Choi\Dropbox\3_program_code\GITHUB\imaginexlab_smartglove\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36BAE08-4BE8-4973-8086-16D696F496B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86292CD1-DCDE-4E79-9BE8-572FA1814B6C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="478" xr2:uid="{DEA0BA13-803F-4C08-A035-B07F2889F4B2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>신희</t>
+  </si>
+  <si>
+    <t>혜민</t>
   </si>
 </sst>
 </file>
@@ -312,7 +315,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -441,21 +444,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -574,12 +562,96 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -590,23 +662,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -616,43 +708,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -663,6 +731,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -982,8 +1059,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1002,17 +1079,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="33"/>
       <c r="J1" t="s">
         <v>17</v>
       </c>
@@ -1021,110 +1098,110 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="36"/>
       <c r="J2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="22">
+      <c r="J3" s="21">
         <v>0</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="17"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="16"/>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="43">
         <v>1992</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="3" t="str">
+      <c r="E4" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="43" t="str">
         <f>CONCATENATE("Hand_IMU_20_",J3+1,".txt")</f>
         <v>Hand_IMU_20_1.txt</v>
       </c>
-      <c r="I4" s="7" t="str">
+      <c r="I4" s="44" t="str">
         <f>CONCATENATE("Wrist_IMU_20_",J3+1,".txt")</f>
         <v>Wrist_IMU_20_1.txt</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="13">
         <f>J3+1</f>
         <v>1</v>
       </c>
       <c r="K4" s="3"/>
-      <c r="N4" s="18" t="s">
+      <c r="N4" s="17" t="s">
         <v>29</v>
       </c>
       <c r="O4" s="2"/>
-      <c r="P4" s="33" t="s">
+      <c r="P4" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="34"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="38"/>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="6" t="s">
@@ -1156,21 +1233,21 @@
         <f t="shared" ref="I5:I22" si="1">CONCATENATE("Wrist_IMU_20_",J4+1,".txt")</f>
         <v>Wrist_IMU_20_2.txt</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="13">
         <f t="shared" ref="J5:J68" si="2">J4+1</f>
         <v>2</v>
       </c>
       <c r="K5" s="3"/>
-      <c r="N5" s="20" t="s">
+      <c r="N5" s="19" t="s">
         <v>8</v>
       </c>
       <c r="O5" s="2"/>
-      <c r="P5" s="35" t="s">
+      <c r="P5" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="36"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="28"/>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="6" t="s">
@@ -1202,21 +1279,21 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_20_3.txt</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="13">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K6" s="3"/>
-      <c r="N6" s="20" t="s">
+      <c r="N6" s="19" t="s">
         <v>2</v>
       </c>
       <c r="O6" s="2"/>
-      <c r="P6" s="35" t="s">
+      <c r="P6" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="36"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="28"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="6" t="s">
@@ -1248,21 +1325,21 @@
         <f>CONCATENATE("Wrist_IMU_20_",J6+1,".txt")</f>
         <v>Wrist_IMU_20_4.txt</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="13">
         <f>J6+1</f>
         <v>4</v>
       </c>
       <c r="K7" s="3"/>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="19" t="s">
         <v>9</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="35" t="s">
+      <c r="P7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="35"/>
-      <c r="S7" s="36"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="28"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="6" t="s">
@@ -1294,21 +1371,21 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_20_5.txt</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="13">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="K8" s="3"/>
-      <c r="N8" s="39" t="s">
+      <c r="N8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="40"/>
-      <c r="P8" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="36"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="28"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="6" t="s">
@@ -1340,19 +1417,19 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_20_6.txt</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="13">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="K9" s="3"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="35" t="s">
+      <c r="N9" s="25"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="36"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="28"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="6" t="s">
@@ -1384,21 +1461,21 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_20_7.txt</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="13">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="K10" s="3"/>
-      <c r="N10" s="20" t="s">
+      <c r="N10" s="19" t="s">
         <v>14</v>
       </c>
       <c r="O10" s="2"/>
-      <c r="P10" s="41">
+      <c r="P10" s="29">
         <v>4.5891203703703705E-2</v>
       </c>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="41"/>
-      <c r="S10" s="42"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="30"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="6" t="s">
@@ -1430,21 +1507,21 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_20_8.txt</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="13">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="K11" s="3"/>
-      <c r="N11" s="20" t="s">
+      <c r="N11" s="19" t="s">
         <v>15</v>
       </c>
       <c r="O11" s="2"/>
-      <c r="P11" s="35" t="s">
+      <c r="P11" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="36"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="28"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1">
       <c r="A12" s="6" t="s">
@@ -1476,21 +1553,21 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_20_9.txt</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="13">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="K12" s="3"/>
-      <c r="N12" s="21" t="s">
+      <c r="N12" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="O12" s="19"/>
-      <c r="P12" s="37" t="s">
+      <c r="O12" s="18"/>
+      <c r="P12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="37"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="38"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="24"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="6" t="s">
@@ -1522,7 +1599,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_20_10.txt</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="13">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
@@ -1558,7 +1635,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_20_11.txt</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="13">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
@@ -1594,7 +1671,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_20_12.txt</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="13">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
@@ -1630,7 +1707,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_20_13.txt</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="13">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
@@ -1673,7 +1750,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_20_14.txt</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="13">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
@@ -1683,7 +1760,7 @@
       </c>
       <c r="O17">
         <f>SUMPRODUCT(LEN(D4:D63)-LEN(SUBSTITUTE(D4:D63,"F","")))</f>
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1716,7 +1793,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_20_15.txt</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="13">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
@@ -1726,7 +1803,7 @@
       </c>
       <c r="O18">
         <f>O17/O16</f>
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1759,7 +1836,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_20_16.txt</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="13">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
@@ -1795,7 +1872,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_20_17.txt</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="13">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
@@ -1831,7 +1908,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_20_18.txt</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="13">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
@@ -1867,7 +1944,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_20_19.txt</v>
       </c>
-      <c r="J22" s="14">
+      <c r="J22" s="13">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
@@ -1903,7 +1980,7 @@
         <f t="shared" ref="I23:I59" si="4">CONCATENATE("Wrist_IMU_20_",J22+1,".txt")</f>
         <v>Wrist_IMU_20_20.txt</v>
       </c>
-      <c r="J23" s="14">
+      <c r="J23" s="13">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
@@ -1939,7 +2016,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_21.txt</v>
       </c>
-      <c r="J24" s="14">
+      <c r="J24" s="13">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
@@ -1975,7 +2052,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_22.txt</v>
       </c>
-      <c r="J25" s="14">
+      <c r="J25" s="13">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
@@ -2011,7 +2088,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_23.txt</v>
       </c>
-      <c r="J26" s="14">
+      <c r="J26" s="13">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
@@ -2047,7 +2124,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_24.txt</v>
       </c>
-      <c r="J27" s="14">
+      <c r="J27" s="13">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
@@ -2083,7 +2160,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_25.txt</v>
       </c>
-      <c r="J28" s="14">
+      <c r="J28" s="13">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
@@ -2119,7 +2196,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_26.txt</v>
       </c>
-      <c r="J29" s="14">
+      <c r="J29" s="13">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
@@ -2155,7 +2232,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_27.txt</v>
       </c>
-      <c r="J30" s="14">
+      <c r="J30" s="13">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
@@ -2191,7 +2268,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_28.txt</v>
       </c>
-      <c r="J31" s="14">
+      <c r="J31" s="13">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
@@ -2227,7 +2304,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_29.txt</v>
       </c>
-      <c r="J32" s="14">
+      <c r="J32" s="13">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
@@ -2263,7 +2340,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_30.txt</v>
       </c>
-      <c r="J33" s="14">
+      <c r="J33" s="13">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
@@ -2299,7 +2376,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_31.txt</v>
       </c>
-      <c r="J34" s="14">
+      <c r="J34" s="13">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
@@ -2335,7 +2412,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_32.txt</v>
       </c>
-      <c r="J35" s="14">
+      <c r="J35" s="13">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
@@ -2371,7 +2448,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_33.txt</v>
       </c>
-      <c r="J36" s="14">
+      <c r="J36" s="13">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
@@ -2407,7 +2484,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_34.txt</v>
       </c>
-      <c r="J37" s="14">
+      <c r="J37" s="13">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
@@ -2443,7 +2520,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_35.txt</v>
       </c>
-      <c r="J38" s="14">
+      <c r="J38" s="13">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
@@ -2479,7 +2556,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_36.txt</v>
       </c>
-      <c r="J39" s="14">
+      <c r="J39" s="13">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
@@ -2515,7 +2592,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_37.txt</v>
       </c>
-      <c r="J40" s="14">
+      <c r="J40" s="13">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
@@ -2551,7 +2628,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_38.txt</v>
       </c>
-      <c r="J41" s="14">
+      <c r="J41" s="13">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
@@ -2587,7 +2664,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_39.txt</v>
       </c>
-      <c r="J42" s="14">
+      <c r="J42" s="13">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
@@ -2623,7 +2700,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_40.txt</v>
       </c>
-      <c r="J43" s="14">
+      <c r="J43" s="13">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
@@ -2659,7 +2736,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_41.txt</v>
       </c>
-      <c r="J44" s="14">
+      <c r="J44" s="13">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
@@ -2695,7 +2772,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_42.txt</v>
       </c>
-      <c r="J45" s="14">
+      <c r="J45" s="13">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
@@ -2731,7 +2808,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_43.txt</v>
       </c>
-      <c r="J46" s="14">
+      <c r="J46" s="13">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
@@ -2767,7 +2844,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_44.txt</v>
       </c>
-      <c r="J47" s="14">
+      <c r="J47" s="13">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
@@ -2803,7 +2880,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_45.txt</v>
       </c>
-      <c r="J48" s="14">
+      <c r="J48" s="13">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
@@ -2839,7 +2916,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_46.txt</v>
       </c>
-      <c r="J49" s="14">
+      <c r="J49" s="13">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
@@ -2875,7 +2952,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_47.txt</v>
       </c>
-      <c r="J50" s="14">
+      <c r="J50" s="13">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
@@ -2911,7 +2988,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_48.txt</v>
       </c>
-      <c r="J51" s="14">
+      <c r="J51" s="13">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
@@ -2947,7 +3024,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_49.txt</v>
       </c>
-      <c r="J52" s="14">
+      <c r="J52" s="13">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
@@ -2983,7 +3060,7 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_50.txt</v>
       </c>
-      <c r="J53" s="14">
+      <c r="J53" s="13">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
@@ -3019,18 +3096,28 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_51.txt</v>
       </c>
-      <c r="J54" s="14">
+      <c r="J54" s="13">
         <f t="shared" si="2"/>
         <v>51</v>
       </c>
       <c r="K54" s="3"/>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="6"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
+      <c r="A55" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" s="3">
+        <v>1994</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F55" s="3" t="s">
         <v>12</v>
       </c>
@@ -3045,18 +3132,28 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_52.txt</v>
       </c>
-      <c r="J55" s="14">
+      <c r="J55" s="13">
         <f t="shared" si="2"/>
         <v>52</v>
       </c>
-      <c r="K55" s="3"/>
+      <c r="K55" s="48"/>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56" s="6"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
+      <c r="A56" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56" s="3">
+        <v>1994</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F56" s="3" t="s">
         <v>12</v>
       </c>
@@ -3071,18 +3168,28 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_53.txt</v>
       </c>
-      <c r="J56" s="14">
+      <c r="J56" s="13">
         <f t="shared" si="2"/>
         <v>53</v>
       </c>
-      <c r="K56" s="3"/>
+      <c r="K56" s="48"/>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" s="6"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
+      <c r="A57" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C57" s="3">
+        <v>1994</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F57" s="3" t="s">
         <v>12</v>
       </c>
@@ -3097,11 +3204,11 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_54.txt</v>
       </c>
-      <c r="J57" s="14">
+      <c r="J57" s="13">
         <f t="shared" si="2"/>
         <v>54</v>
       </c>
-      <c r="K57" s="3"/>
+      <c r="K57" s="48"/>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="6"/>
@@ -3123,533 +3230,1293 @@
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_55.txt</v>
       </c>
-      <c r="J58" s="14">
+      <c r="J58" s="13">
         <f t="shared" si="2"/>
         <v>55</v>
       </c>
-      <c r="K58" s="3"/>
-    </row>
-    <row r="59" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A59" s="8"/>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
+      <c r="K58" s="48"/>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="6"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
       <c r="D59" s="3"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H59" s="9" t="str">
+      <c r="E59" s="3"/>
+      <c r="F59" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H59" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Hand_IMU_20_56.txt</v>
       </c>
-      <c r="I59" s="10" t="str">
+      <c r="I59" s="7" t="str">
         <f t="shared" si="4"/>
         <v>Wrist_IMU_20_56.txt</v>
       </c>
-      <c r="J59" s="14">
+      <c r="J59" s="13">
         <f t="shared" si="2"/>
         <v>56</v>
       </c>
       <c r="K59" s="3"/>
     </row>
-    <row r="60" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A60" s="8"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
+    <row r="60" spans="1:11">
+      <c r="A60" s="6"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
       <c r="D60" s="3"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H60" s="9" t="str">
+      <c r="E60" s="3"/>
+      <c r="F60" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H60" s="3" t="str">
         <f t="shared" ref="H60:H63" si="5">CONCATENATE("Hand_IMU_20_",J59+1,".txt")</f>
         <v>Hand_IMU_20_57.txt</v>
       </c>
-      <c r="I60" s="10" t="str">
+      <c r="I60" s="7" t="str">
         <f t="shared" ref="I60:I63" si="6">CONCATENATE("Wrist_IMU_20_",J59+1,".txt")</f>
         <v>Wrist_IMU_20_57.txt</v>
       </c>
-      <c r="J60" s="14">
+      <c r="J60" s="13">
         <f t="shared" si="2"/>
         <v>57</v>
       </c>
       <c r="K60" s="3"/>
     </row>
-    <row r="61" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A61" s="8"/>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H61" s="9" t="str">
+    <row r="61" spans="1:11">
+      <c r="A61" s="6"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H61" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Hand_IMU_20_58.txt</v>
       </c>
-      <c r="I61" s="10" t="str">
+      <c r="I61" s="7" t="str">
         <f t="shared" si="6"/>
         <v>Wrist_IMU_20_58.txt</v>
       </c>
-      <c r="J61" s="14">
+      <c r="J61" s="13">
         <f t="shared" si="2"/>
         <v>58</v>
       </c>
       <c r="K61" s="3"/>
     </row>
-    <row r="62" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A62" s="8"/>
-      <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G62" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H62" s="9" t="str">
+    <row r="62" spans="1:11">
+      <c r="A62" s="6"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H62" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Hand_IMU_20_59.txt</v>
       </c>
-      <c r="I62" s="10" t="str">
+      <c r="I62" s="7" t="str">
         <f t="shared" si="6"/>
         <v>Wrist_IMU_20_59.txt</v>
       </c>
-      <c r="J62" s="14">
+      <c r="J62" s="13">
         <f t="shared" si="2"/>
         <v>59</v>
       </c>
       <c r="K62" s="3"/>
     </row>
-    <row r="63" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A63" s="8"/>
-      <c r="B63" s="9"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G63" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H63" s="9" t="str">
-        <f t="shared" si="5"/>
+    <row r="63" spans="1:11">
+      <c r="A63" s="6"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H63" s="3" t="str">
+        <f t="shared" ref="H63:H72" si="7">CONCATENATE("Hand_IMU_20_",J62+1,".txt")</f>
         <v>Hand_IMU_20_60.txt</v>
       </c>
-      <c r="I63" s="10" t="str">
-        <f t="shared" si="6"/>
+      <c r="I63" s="7" t="str">
+        <f t="shared" ref="I63:I72" si="8">CONCATENATE("Wrist_IMU_20_",J62+1,".txt")</f>
         <v>Wrist_IMU_20_60.txt</v>
       </c>
-      <c r="J63" s="14">
+      <c r="J63" s="13">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="K63" s="3"/>
     </row>
     <row r="64" spans="1:11">
-      <c r="J64" s="14">
+      <c r="A64" s="6"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H64" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>Hand_IMU_20_61.txt</v>
+      </c>
+      <c r="I64" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>Wrist_IMU_20_61.txt</v>
+      </c>
+      <c r="J64" s="13">
         <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="K64" s="3"/>
     </row>
-    <row r="65" spans="10:11">
-      <c r="J65" s="14">
+    <row r="65" spans="1:11">
+      <c r="A65" s="6"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H65" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>Hand_IMU_20_62.txt</v>
+      </c>
+      <c r="I65" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>Wrist_IMU_20_62.txt</v>
+      </c>
+      <c r="J65" s="13">
         <f t="shared" si="2"/>
         <v>62</v>
       </c>
       <c r="K65" s="3"/>
     </row>
-    <row r="66" spans="10:11">
-      <c r="J66" s="14">
+    <row r="66" spans="1:11">
+      <c r="A66" s="6"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H66" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>Hand_IMU_20_63.txt</v>
+      </c>
+      <c r="I66" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>Wrist_IMU_20_63.txt</v>
+      </c>
+      <c r="J66" s="13">
         <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="K66" s="3"/>
     </row>
-    <row r="67" spans="10:11">
-      <c r="J67" s="14">
+    <row r="67" spans="1:11">
+      <c r="A67" s="6"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H67" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>Hand_IMU_20_64.txt</v>
+      </c>
+      <c r="I67" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>Wrist_IMU_20_64.txt</v>
+      </c>
+      <c r="J67" s="13">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="K67" s="3"/>
     </row>
-    <row r="68" spans="10:11">
-      <c r="J68" s="14">
+    <row r="68" spans="1:11">
+      <c r="A68" s="6"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H68" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>Hand_IMU_20_65.txt</v>
+      </c>
+      <c r="I68" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>Wrist_IMU_20_65.txt</v>
+      </c>
+      <c r="J68" s="13">
         <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="K68" s="3"/>
     </row>
-    <row r="69" spans="10:11">
-      <c r="J69" s="14">
-        <f t="shared" ref="J69:J117" si="7">J68+1</f>
+    <row r="69" spans="1:11">
+      <c r="A69" s="6"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H69" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>Hand_IMU_20_66.txt</v>
+      </c>
+      <c r="I69" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>Wrist_IMU_20_66.txt</v>
+      </c>
+      <c r="J69" s="13">
+        <f t="shared" ref="J69:J117" si="9">J68+1</f>
         <v>66</v>
       </c>
       <c r="K69" s="3"/>
     </row>
-    <row r="70" spans="10:11">
-      <c r="J70" s="14">
+    <row r="70" spans="1:11">
+      <c r="A70" s="6"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H70" s="3" t="str">
         <f t="shared" si="7"/>
+        <v>Hand_IMU_20_67.txt</v>
+      </c>
+      <c r="I70" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>Wrist_IMU_20_67.txt</v>
+      </c>
+      <c r="J70" s="13">
+        <f t="shared" si="9"/>
         <v>67</v>
       </c>
       <c r="K70" s="3"/>
     </row>
-    <row r="71" spans="10:11">
-      <c r="J71" s="14">
+    <row r="71" spans="1:11">
+      <c r="A71" s="6"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H71" s="3" t="str">
         <f t="shared" si="7"/>
+        <v>Hand_IMU_20_68.txt</v>
+      </c>
+      <c r="I71" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>Wrist_IMU_20_68.txt</v>
+      </c>
+      <c r="J71" s="13">
+        <f t="shared" si="9"/>
         <v>68</v>
       </c>
       <c r="K71" s="3"/>
     </row>
-    <row r="72" spans="10:11">
-      <c r="J72" s="14">
+    <row r="72" spans="1:11">
+      <c r="A72" s="6"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H72" s="3" t="str">
         <f t="shared" si="7"/>
+        <v>Hand_IMU_20_69.txt</v>
+      </c>
+      <c r="I72" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>Wrist_IMU_20_69.txt</v>
+      </c>
+      <c r="J72" s="13">
+        <f t="shared" si="9"/>
         <v>69</v>
       </c>
       <c r="K72" s="3"/>
     </row>
-    <row r="73" spans="10:11">
-      <c r="J73" s="14">
-        <f t="shared" si="7"/>
+    <row r="73" spans="1:11">
+      <c r="A73" s="6"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H73" s="3" t="str">
+        <f t="shared" ref="H73:H103" si="10">CONCATENATE("Hand_IMU_20_",J72+1,".txt")</f>
+        <v>Hand_IMU_20_70.txt</v>
+      </c>
+      <c r="I73" s="7" t="str">
+        <f t="shared" ref="I73:I103" si="11">CONCATENATE("Wrist_IMU_20_",J72+1,".txt")</f>
+        <v>Wrist_IMU_20_70.txt</v>
+      </c>
+      <c r="J73" s="13">
+        <f t="shared" si="9"/>
         <v>70</v>
       </c>
       <c r="K73" s="3"/>
     </row>
-    <row r="74" spans="10:11">
-      <c r="J74" s="14">
-        <f t="shared" si="7"/>
+    <row r="74" spans="1:11">
+      <c r="A74" s="6"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H74" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_71.txt</v>
+      </c>
+      <c r="I74" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_71.txt</v>
+      </c>
+      <c r="J74" s="13">
+        <f t="shared" si="9"/>
         <v>71</v>
       </c>
       <c r="K74" s="3"/>
     </row>
-    <row r="75" spans="10:11">
-      <c r="J75" s="14">
-        <f t="shared" si="7"/>
+    <row r="75" spans="1:11">
+      <c r="A75" s="6"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H75" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_72.txt</v>
+      </c>
+      <c r="I75" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_72.txt</v>
+      </c>
+      <c r="J75" s="13">
+        <f t="shared" si="9"/>
         <v>72</v>
       </c>
       <c r="K75" s="3"/>
     </row>
-    <row r="76" spans="10:11">
-      <c r="J76" s="14">
-        <f t="shared" si="7"/>
+    <row r="76" spans="1:11">
+      <c r="A76" s="6"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H76" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_73.txt</v>
+      </c>
+      <c r="I76" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_73.txt</v>
+      </c>
+      <c r="J76" s="13">
+        <f t="shared" si="9"/>
         <v>73</v>
       </c>
       <c r="K76" s="3"/>
     </row>
-    <row r="77" spans="10:11">
-      <c r="J77" s="14">
-        <f t="shared" si="7"/>
+    <row r="77" spans="1:11">
+      <c r="A77" s="6"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H77" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_74.txt</v>
+      </c>
+      <c r="I77" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_74.txt</v>
+      </c>
+      <c r="J77" s="13">
+        <f t="shared" si="9"/>
         <v>74</v>
       </c>
       <c r="K77" s="3"/>
     </row>
-    <row r="78" spans="10:11">
-      <c r="J78" s="14">
-        <f t="shared" si="7"/>
+    <row r="78" spans="1:11">
+      <c r="A78" s="6"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H78" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_75.txt</v>
+      </c>
+      <c r="I78" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_75.txt</v>
+      </c>
+      <c r="J78" s="13">
+        <f t="shared" si="9"/>
         <v>75</v>
       </c>
       <c r="K78" s="3"/>
     </row>
-    <row r="79" spans="10:11">
-      <c r="J79" s="14">
-        <f t="shared" si="7"/>
+    <row r="79" spans="1:11">
+      <c r="A79" s="6"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H79" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_76.txt</v>
+      </c>
+      <c r="I79" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_76.txt</v>
+      </c>
+      <c r="J79" s="13">
+        <f t="shared" si="9"/>
         <v>76</v>
       </c>
       <c r="K79" s="3"/>
     </row>
-    <row r="80" spans="10:11">
-      <c r="J80" s="14">
-        <f t="shared" si="7"/>
+    <row r="80" spans="1:11">
+      <c r="A80" s="6"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H80" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_77.txt</v>
+      </c>
+      <c r="I80" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_77.txt</v>
+      </c>
+      <c r="J80" s="13">
+        <f t="shared" si="9"/>
         <v>77</v>
       </c>
       <c r="K80" s="3"/>
     </row>
-    <row r="81" spans="10:11">
-      <c r="J81" s="14">
-        <f t="shared" si="7"/>
+    <row r="81" spans="1:11">
+      <c r="A81" s="6"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H81" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_78.txt</v>
+      </c>
+      <c r="I81" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_78.txt</v>
+      </c>
+      <c r="J81" s="13">
+        <f t="shared" si="9"/>
         <v>78</v>
       </c>
       <c r="K81" s="3"/>
     </row>
-    <row r="82" spans="10:11">
-      <c r="J82" s="14">
-        <f t="shared" si="7"/>
+    <row r="82" spans="1:11">
+      <c r="A82" s="6"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H82" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_79.txt</v>
+      </c>
+      <c r="I82" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_79.txt</v>
+      </c>
+      <c r="J82" s="13">
+        <f t="shared" si="9"/>
         <v>79</v>
       </c>
       <c r="K82" s="3"/>
     </row>
-    <row r="83" spans="10:11">
-      <c r="J83" s="14">
-        <f t="shared" si="7"/>
+    <row r="83" spans="1:11">
+      <c r="A83" s="6"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H83" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_80.txt</v>
+      </c>
+      <c r="I83" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_80.txt</v>
+      </c>
+      <c r="J83" s="13">
+        <f t="shared" si="9"/>
         <v>80</v>
       </c>
       <c r="K83" s="3"/>
     </row>
-    <row r="84" spans="10:11">
-      <c r="J84" s="14">
-        <f t="shared" si="7"/>
+    <row r="84" spans="1:11">
+      <c r="A84" s="6"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H84" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_81.txt</v>
+      </c>
+      <c r="I84" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_81.txt</v>
+      </c>
+      <c r="J84" s="13">
+        <f t="shared" si="9"/>
         <v>81</v>
       </c>
       <c r="K84" s="3"/>
     </row>
-    <row r="85" spans="10:11">
-      <c r="J85" s="14">
-        <f t="shared" si="7"/>
+    <row r="85" spans="1:11">
+      <c r="A85" s="6"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H85" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_82.txt</v>
+      </c>
+      <c r="I85" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_82.txt</v>
+      </c>
+      <c r="J85" s="13">
+        <f t="shared" si="9"/>
         <v>82</v>
       </c>
       <c r="K85" s="3"/>
     </row>
-    <row r="86" spans="10:11">
-      <c r="J86" s="14">
-        <f t="shared" si="7"/>
+    <row r="86" spans="1:11">
+      <c r="A86" s="6"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H86" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_83.txt</v>
+      </c>
+      <c r="I86" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_83.txt</v>
+      </c>
+      <c r="J86" s="13">
+        <f t="shared" si="9"/>
         <v>83</v>
       </c>
       <c r="K86" s="3"/>
     </row>
-    <row r="87" spans="10:11">
-      <c r="J87" s="14">
-        <f t="shared" si="7"/>
+    <row r="87" spans="1:11">
+      <c r="A87" s="6"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H87" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_84.txt</v>
+      </c>
+      <c r="I87" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_84.txt</v>
+      </c>
+      <c r="J87" s="13">
+        <f t="shared" si="9"/>
         <v>84</v>
       </c>
       <c r="K87" s="3"/>
     </row>
-    <row r="88" spans="10:11">
-      <c r="J88" s="14">
-        <f t="shared" si="7"/>
+    <row r="88" spans="1:11">
+      <c r="A88" s="6"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H88" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_85.txt</v>
+      </c>
+      <c r="I88" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_85.txt</v>
+      </c>
+      <c r="J88" s="13">
+        <f t="shared" si="9"/>
         <v>85</v>
       </c>
       <c r="K88" s="3"/>
     </row>
-    <row r="89" spans="10:11">
-      <c r="J89" s="14">
-        <f t="shared" si="7"/>
+    <row r="89" spans="1:11">
+      <c r="A89" s="6"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H89" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_86.txt</v>
+      </c>
+      <c r="I89" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_86.txt</v>
+      </c>
+      <c r="J89" s="13">
+        <f t="shared" si="9"/>
         <v>86</v>
       </c>
       <c r="K89" s="3"/>
     </row>
-    <row r="90" spans="10:11">
-      <c r="J90" s="14">
-        <f t="shared" si="7"/>
+    <row r="90" spans="1:11">
+      <c r="A90" s="6"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H90" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_87.txt</v>
+      </c>
+      <c r="I90" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_87.txt</v>
+      </c>
+      <c r="J90" s="13">
+        <f t="shared" si="9"/>
         <v>87</v>
       </c>
       <c r="K90" s="3"/>
     </row>
-    <row r="91" spans="10:11">
-      <c r="J91" s="14">
-        <f t="shared" si="7"/>
+    <row r="91" spans="1:11">
+      <c r="A91" s="6"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H91" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_88.txt</v>
+      </c>
+      <c r="I91" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_88.txt</v>
+      </c>
+      <c r="J91" s="13">
+        <f t="shared" si="9"/>
         <v>88</v>
       </c>
       <c r="K91" s="3"/>
     </row>
-    <row r="92" spans="10:11">
-      <c r="J92" s="14">
-        <f t="shared" si="7"/>
+    <row r="92" spans="1:11">
+      <c r="A92" s="6"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H92" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_89.txt</v>
+      </c>
+      <c r="I92" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_89.txt</v>
+      </c>
+      <c r="J92" s="13">
+        <f t="shared" si="9"/>
         <v>89</v>
       </c>
       <c r="K92" s="3"/>
     </row>
-    <row r="93" spans="10:11">
-      <c r="J93" s="14">
-        <f t="shared" si="7"/>
+    <row r="93" spans="1:11">
+      <c r="A93" s="6"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H93" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_90.txt</v>
+      </c>
+      <c r="I93" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_90.txt</v>
+      </c>
+      <c r="J93" s="13">
+        <f t="shared" si="9"/>
         <v>90</v>
       </c>
       <c r="K93" s="3"/>
     </row>
-    <row r="94" spans="10:11">
-      <c r="J94" s="14">
-        <f t="shared" si="7"/>
+    <row r="94" spans="1:11">
+      <c r="A94" s="6"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H94" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_91.txt</v>
+      </c>
+      <c r="I94" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_91.txt</v>
+      </c>
+      <c r="J94" s="13">
+        <f t="shared" si="9"/>
         <v>91</v>
       </c>
       <c r="K94" s="3"/>
     </row>
-    <row r="95" spans="10:11">
-      <c r="J95" s="14">
-        <f t="shared" si="7"/>
+    <row r="95" spans="1:11">
+      <c r="A95" s="6"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H95" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_92.txt</v>
+      </c>
+      <c r="I95" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_92.txt</v>
+      </c>
+      <c r="J95" s="13">
+        <f t="shared" si="9"/>
         <v>92</v>
       </c>
       <c r="K95" s="3"/>
     </row>
-    <row r="96" spans="10:11">
-      <c r="J96" s="14">
-        <f t="shared" si="7"/>
+    <row r="96" spans="1:11">
+      <c r="A96" s="6"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H96" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_93.txt</v>
+      </c>
+      <c r="I96" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_93.txt</v>
+      </c>
+      <c r="J96" s="13">
+        <f t="shared" si="9"/>
         <v>93</v>
       </c>
       <c r="K96" s="3"/>
     </row>
-    <row r="97" spans="10:11">
-      <c r="J97" s="14">
-        <f t="shared" si="7"/>
+    <row r="97" spans="1:11">
+      <c r="A97" s="6"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H97" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_94.txt</v>
+      </c>
+      <c r="I97" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_94.txt</v>
+      </c>
+      <c r="J97" s="13">
+        <f t="shared" si="9"/>
         <v>94</v>
       </c>
       <c r="K97" s="3"/>
     </row>
-    <row r="98" spans="10:11">
-      <c r="J98" s="14">
-        <f t="shared" si="7"/>
+    <row r="98" spans="1:11">
+      <c r="A98" s="6"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H98" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_95.txt</v>
+      </c>
+      <c r="I98" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_95.txt</v>
+      </c>
+      <c r="J98" s="13">
+        <f t="shared" si="9"/>
         <v>95</v>
       </c>
       <c r="K98" s="3"/>
     </row>
-    <row r="99" spans="10:11">
-      <c r="J99" s="14">
-        <f t="shared" si="7"/>
+    <row r="99" spans="1:11">
+      <c r="A99" s="6"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H99" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_96.txt</v>
+      </c>
+      <c r="I99" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_96.txt</v>
+      </c>
+      <c r="J99" s="13">
+        <f t="shared" si="9"/>
         <v>96</v>
       </c>
       <c r="K99" s="3"/>
     </row>
-    <row r="100" spans="10:11">
-      <c r="J100" s="14">
-        <f t="shared" si="7"/>
+    <row r="100" spans="1:11">
+      <c r="A100" s="6"/>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H100" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_97.txt</v>
+      </c>
+      <c r="I100" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_97.txt</v>
+      </c>
+      <c r="J100" s="13">
+        <f t="shared" si="9"/>
         <v>97</v>
       </c>
       <c r="K100" s="3"/>
     </row>
-    <row r="101" spans="10:11">
-      <c r="J101" s="14">
-        <f t="shared" si="7"/>
+    <row r="101" spans="1:11">
+      <c r="A101" s="6"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H101" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_98.txt</v>
+      </c>
+      <c r="I101" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_98.txt</v>
+      </c>
+      <c r="J101" s="13">
+        <f t="shared" si="9"/>
         <v>98</v>
       </c>
       <c r="K101" s="3"/>
     </row>
-    <row r="102" spans="10:11">
-      <c r="J102" s="14">
-        <f t="shared" si="7"/>
+    <row r="102" spans="1:11">
+      <c r="A102" s="6"/>
+      <c r="B102" s="3"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H102" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_99.txt</v>
+      </c>
+      <c r="I102" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_99.txt</v>
+      </c>
+      <c r="J102" s="13">
+        <f t="shared" si="9"/>
         <v>99</v>
       </c>
       <c r="K102" s="3"/>
     </row>
-    <row r="103" spans="10:11">
-      <c r="J103" s="14">
-        <f t="shared" si="7"/>
+    <row r="103" spans="1:11">
+      <c r="A103" s="6"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H103" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>Hand_IMU_20_100.txt</v>
+      </c>
+      <c r="I103" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>Wrist_IMU_20_100.txt</v>
+      </c>
+      <c r="J103" s="13">
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="K103" s="3"/>
     </row>
-    <row r="104" spans="10:11">
-      <c r="J104" s="14">
-        <f t="shared" si="7"/>
+    <row r="104" spans="1:11">
+      <c r="J104" s="13">
+        <f t="shared" si="9"/>
         <v>101</v>
       </c>
       <c r="K104" s="3"/>
     </row>
-    <row r="105" spans="10:11">
-      <c r="J105" s="14">
-        <f t="shared" si="7"/>
+    <row r="105" spans="1:11">
+      <c r="J105" s="13">
+        <f t="shared" si="9"/>
         <v>102</v>
       </c>
       <c r="K105" s="3"/>
     </row>
-    <row r="106" spans="10:11">
-      <c r="J106" s="14">
-        <f t="shared" si="7"/>
+    <row r="106" spans="1:11">
+      <c r="J106" s="13">
+        <f t="shared" si="9"/>
         <v>103</v>
       </c>
       <c r="K106" s="3"/>
     </row>
-    <row r="107" spans="10:11">
-      <c r="J107" s="14">
-        <f t="shared" si="7"/>
+    <row r="107" spans="1:11">
+      <c r="J107" s="13">
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
       <c r="K107" s="3"/>
     </row>
-    <row r="108" spans="10:11">
-      <c r="J108" s="14">
-        <f t="shared" si="7"/>
+    <row r="108" spans="1:11">
+      <c r="J108" s="13">
+        <f t="shared" si="9"/>
         <v>105</v>
       </c>
       <c r="K108" s="3"/>
     </row>
-    <row r="109" spans="10:11">
-      <c r="J109" s="14">
-        <f t="shared" si="7"/>
+    <row r="109" spans="1:11">
+      <c r="J109" s="13">
+        <f t="shared" si="9"/>
         <v>106</v>
       </c>
       <c r="K109" s="3"/>
     </row>
-    <row r="110" spans="10:11">
-      <c r="J110" s="14">
-        <f t="shared" si="7"/>
+    <row r="110" spans="1:11">
+      <c r="J110" s="13">
+        <f t="shared" si="9"/>
         <v>107</v>
       </c>
       <c r="K110" s="3"/>
     </row>
-    <row r="111" spans="10:11">
-      <c r="J111" s="14">
-        <f t="shared" si="7"/>
+    <row r="111" spans="1:11">
+      <c r="J111" s="13">
+        <f t="shared" si="9"/>
         <v>108</v>
       </c>
       <c r="K111" s="3"/>
     </row>
-    <row r="112" spans="10:11">
-      <c r="J112" s="14">
-        <f t="shared" si="7"/>
+    <row r="112" spans="1:11">
+      <c r="J112" s="13">
+        <f t="shared" si="9"/>
         <v>109</v>
       </c>
       <c r="K112" s="3"/>
     </row>
     <row r="113" spans="10:11">
-      <c r="J113" s="14">
-        <f t="shared" si="7"/>
+      <c r="J113" s="13">
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="K113" s="3"/>
     </row>
     <row r="114" spans="10:11">
-      <c r="J114" s="14">
-        <f t="shared" si="7"/>
+      <c r="J114" s="13">
+        <f t="shared" si="9"/>
         <v>111</v>
       </c>
       <c r="K114" s="3"/>
     </row>
     <row r="115" spans="10:11">
-      <c r="J115" s="14">
-        <f t="shared" si="7"/>
+      <c r="J115" s="13">
+        <f t="shared" si="9"/>
         <v>112</v>
       </c>
       <c r="K115" s="3"/>
     </row>
     <row r="116" spans="10:11">
-      <c r="J116" s="14">
-        <f t="shared" si="7"/>
+      <c r="J116" s="13">
+        <f t="shared" si="9"/>
         <v>113</v>
       </c>
       <c r="K116" s="3"/>
     </row>
     <row r="117" spans="10:11">
-      <c r="J117" s="14">
-        <f t="shared" si="7"/>
+      <c r="J117" s="13">
+        <f t="shared" si="9"/>
         <v>114</v>
       </c>
       <c r="K117" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="P7:S7"/>
     <mergeCell ref="P12:S12"/>
     <mergeCell ref="N8:O9"/>
     <mergeCell ref="P8:S8"/>
     <mergeCell ref="P9:S9"/>
     <mergeCell ref="P10:S10"/>
     <mergeCell ref="P11:S11"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="P5:S5"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="P7:S7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3681,31 +4548,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="33"/>
       <c r="J1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A2" s="43"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="45"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="41"/>
       <c r="J2" t="s">
         <v>18</v>
       </c>
@@ -3738,23 +4605,23 @@
       <c r="I3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="22">
+      <c r="J3" s="21">
         <v>0</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="17"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="16"/>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="6"/>
@@ -3772,23 +4639,23 @@
         <f>CONCATENATE("Wrist_IMU_60_",J3+1,".txt")</f>
         <v>Wrist_IMU_60_1.txt</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="13">
         <f>J3+1</f>
         <v>1</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="18" t="s">
+      <c r="N4" s="17" t="s">
         <v>29</v>
       </c>
       <c r="O4" s="2"/>
-      <c r="P4" s="33" t="s">
+      <c r="P4" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="34"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="38"/>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="6"/>
@@ -3797,7 +4664,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="12"/>
+      <c r="G5" s="11"/>
       <c r="H5" s="3" t="str">
         <f t="shared" ref="H5:H22" si="0">CONCATENATE("Hand_IMU_60_",J4+1,".txt")</f>
         <v>Hand_IMU_60_2.txt</v>
@@ -3806,21 +4673,21 @@
         <f t="shared" ref="I5:I22" si="1">CONCATENATE("Wrist_IMU_60_",J4+1,".txt")</f>
         <v>Wrist_IMU_60_2.txt</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="13">
         <f t="shared" ref="J5:J22" si="2">J4+1</f>
         <v>2</v>
       </c>
       <c r="K5" s="3"/>
-      <c r="N5" s="20" t="s">
+      <c r="N5" s="19" t="s">
         <v>8</v>
       </c>
       <c r="O5" s="2"/>
-      <c r="P5" s="35" t="s">
+      <c r="P5" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="36"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="28"/>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="6"/>
@@ -3829,7 +4696,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="12"/>
+      <c r="G6" s="11"/>
       <c r="H6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_3.txt</v>
@@ -3838,21 +4705,21 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_3.txt</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="13">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K6" s="3"/>
-      <c r="N6" s="20" t="s">
+      <c r="N6" s="19" t="s">
         <v>2</v>
       </c>
       <c r="O6" s="2"/>
-      <c r="P6" s="35" t="s">
+      <c r="P6" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="36"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="28"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="6"/>
@@ -3861,7 +4728,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="12"/>
+      <c r="G7" s="11"/>
       <c r="H7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_4.txt</v>
@@ -3870,21 +4737,21 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_4.txt</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="13">
         <f>J6+1</f>
         <v>4</v>
       </c>
       <c r="K7" s="3"/>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="19" t="s">
         <v>9</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="35" t="s">
+      <c r="P7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="35"/>
-      <c r="S7" s="36"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="28"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="6"/>
@@ -3893,7 +4760,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="12"/>
+      <c r="G8" s="11"/>
       <c r="H8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_5.txt</v>
@@ -3902,21 +4769,21 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_5.txt</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="13">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="K8" s="3"/>
-      <c r="N8" s="39" t="s">
+      <c r="N8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="40"/>
-      <c r="P8" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="36"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="28"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="6"/>
@@ -3925,7 +4792,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="12"/>
+      <c r="G9" s="11"/>
       <c r="H9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_6.txt</v>
@@ -3934,19 +4801,19 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_6.txt</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="13">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="K9" s="3"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="35" t="s">
+      <c r="N9" s="25"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="36"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="28"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="6"/>
@@ -3955,7 +4822,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="12"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_7.txt</v>
@@ -3964,21 +4831,21 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_7.txt</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="13">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="K10" s="3"/>
-      <c r="N10" s="20" t="s">
+      <c r="N10" s="19" t="s">
         <v>14</v>
       </c>
       <c r="O10" s="2"/>
-      <c r="P10" s="41">
+      <c r="P10" s="29">
         <v>4.5891203703703705E-2</v>
       </c>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="41"/>
-      <c r="S10" s="42"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="30"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="6"/>
@@ -3987,7 +4854,7 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="12"/>
+      <c r="G11" s="11"/>
       <c r="H11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_8.txt</v>
@@ -3996,21 +4863,21 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_8.txt</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="13">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="K11" s="3"/>
-      <c r="N11" s="20" t="s">
+      <c r="N11" s="19" t="s">
         <v>15</v>
       </c>
       <c r="O11" s="2"/>
-      <c r="P11" s="35" t="s">
+      <c r="P11" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="36"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="28"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1">
       <c r="A12" s="6"/>
@@ -4019,7 +4886,7 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="12"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_9.txt</v>
@@ -4028,21 +4895,21 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_9.txt</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="13">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="K12" s="3"/>
-      <c r="N12" s="21" t="s">
+      <c r="N12" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="O12" s="19"/>
-      <c r="P12" s="37" t="s">
+      <c r="O12" s="18"/>
+      <c r="P12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="37"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="38"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="24"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="6"/>
@@ -4051,7 +4918,7 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="12"/>
+      <c r="G13" s="11"/>
       <c r="H13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_10.txt</v>
@@ -4060,7 +4927,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_10.txt</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="13">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
@@ -4073,7 +4940,7 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="12"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_11.txt</v>
@@ -4082,7 +4949,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_11.txt</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="13">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
@@ -4095,7 +4962,7 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="12"/>
+      <c r="G15" s="11"/>
       <c r="H15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_12.txt</v>
@@ -4104,7 +4971,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_12.txt</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="13">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
@@ -4117,7 +4984,7 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="12"/>
+      <c r="G16" s="11"/>
       <c r="H16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_13.txt</v>
@@ -4126,7 +4993,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_13.txt</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="13">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
@@ -4139,7 +5006,7 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="12"/>
+      <c r="G17" s="11"/>
       <c r="H17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_14.txt</v>
@@ -4148,7 +5015,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_14.txt</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="13">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
@@ -4161,7 +5028,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="12"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_15.txt</v>
@@ -4170,7 +5037,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_15.txt</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="13">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
@@ -4183,7 +5050,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="12"/>
+      <c r="G19" s="11"/>
       <c r="H19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_16.txt</v>
@@ -4192,7 +5059,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_16.txt</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="13">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
@@ -4205,7 +5072,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="12"/>
+      <c r="G20" s="11"/>
       <c r="H20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_17.txt</v>
@@ -4214,7 +5081,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_17.txt</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="13">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
@@ -4227,7 +5094,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="12"/>
+      <c r="G21" s="11"/>
       <c r="H21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_18.txt</v>
@@ -4236,7 +5103,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_18.txt</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="13">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
@@ -4249,7 +5116,7 @@
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="13"/>
+      <c r="G22" s="12"/>
       <c r="H22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Hand_IMU_60_19.txt</v>
@@ -4258,7 +5125,7 @@
         <f t="shared" si="1"/>
         <v>Wrist_IMU_60_19.txt</v>
       </c>
-      <c r="J22" s="14">
+      <c r="J22" s="13">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
feature extraction modification ongoing
</commit_message>
<xml_diff>
--- a/smartglove_data_form.xlsx
+++ b/smartglove_data_form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kanghae Choi\Dropbox\3_program_code\GITHUB\imaginexlab_smartglove\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7712A2DF-7713-4D40-831E-56E443B6C4F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BB0B46-9BC5-48A8-88D8-2862AE588B0A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="478" activeTab="1" xr2:uid="{DEA0BA13-803F-4C08-A035-B07F2889F4B2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="478" activeTab="1" xr2:uid="{DEA0BA13-803F-4C08-A035-B07F2889F4B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Data 20s" sheetId="1" r:id="rId1"/>
@@ -295,9 +295,6 @@
     <t>서운</t>
   </si>
   <si>
-    <t>Paralized and swollen</t>
-  </si>
-  <si>
     <t>순자</t>
   </si>
   <si>
@@ -310,15 +307,9 @@
     <t>NaN</t>
   </si>
   <si>
-    <t>Degenerative Arthrisis</t>
-  </si>
-  <si>
     <t>희남</t>
   </si>
   <si>
-    <t>Rheumatism</t>
-  </si>
-  <si>
     <t>정희</t>
   </si>
   <si>
@@ -331,13 +322,24 @@
     <t>하루자</t>
   </si>
   <si>
-    <t>Swell</t>
-  </si>
-  <si>
     <t>정순</t>
   </si>
   <si>
     <t>Last test on 21 of June 2019</t>
+  </si>
+  <si>
+    <t>Swollen</t>
+  </si>
+  <si>
+    <t>Rheumatoid 
+arthritis</t>
+  </si>
+  <si>
+    <t>Degenerative 
+arthritis</t>
+  </si>
+  <si>
+    <t>Numbed and swollen</t>
   </si>
 </sst>
 </file>
@@ -804,6 +806,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -828,37 +864,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -867,12 +875,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1212,17 +1214,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="45"/>
       <c r="J1" t="s">
         <v>17</v>
       </c>
@@ -1231,15 +1233,15 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="48"/>
       <c r="J2" t="s">
         <v>18</v>
       </c>
@@ -1329,12 +1331,12 @@
         <v>28</v>
       </c>
       <c r="O4" s="2"/>
-      <c r="P4" s="33" t="s">
+      <c r="P4" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="34"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="50"/>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="4" t="s">
@@ -1375,12 +1377,12 @@
         <v>8</v>
       </c>
       <c r="O5" s="2"/>
-      <c r="P5" s="35" t="s">
+      <c r="P5" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="36"/>
+      <c r="Q5" s="39"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="40"/>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="4" t="s">
@@ -1421,12 +1423,12 @@
         <v>2</v>
       </c>
       <c r="O6" s="2"/>
-      <c r="P6" s="35" t="s">
+      <c r="P6" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="36"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="40"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="4" t="s">
@@ -1467,12 +1469,12 @@
         <v>9</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="35" t="s">
+      <c r="P7" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="35"/>
-      <c r="S7" s="36"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="40"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="4" t="s">
@@ -1509,16 +1511,16 @@
         <v>5</v>
       </c>
       <c r="K8" s="3"/>
-      <c r="N8" s="39" t="s">
+      <c r="N8" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="40"/>
-      <c r="P8" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="36"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="40"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="4" t="s">
@@ -1555,14 +1557,14 @@
         <v>6</v>
       </c>
       <c r="K9" s="3"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="35" t="s">
+      <c r="N9" s="37"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="36"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="39"/>
+      <c r="S9" s="40"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="4" t="s">
@@ -1649,12 +1651,12 @@
         <v>15</v>
       </c>
       <c r="O11" s="2"/>
-      <c r="P11" s="35" t="s">
+      <c r="P11" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="36"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="40"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1">
       <c r="A12" s="4" t="s">
@@ -1695,12 +1697,12 @@
         <v>16</v>
       </c>
       <c r="O12" s="15"/>
-      <c r="P12" s="37" t="s">
+      <c r="P12" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="37"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="38"/>
+      <c r="Q12" s="35"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="36"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="4" t="s">
@@ -4639,17 +4641,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="P7:S7"/>
     <mergeCell ref="P12:S12"/>
     <mergeCell ref="N8:O9"/>
     <mergeCell ref="P8:S8"/>
     <mergeCell ref="P9:S9"/>
     <mergeCell ref="P10:S10"/>
     <mergeCell ref="P11:S11"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="P5:S5"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="P7:S7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4661,8 +4663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E86554-00CB-4203-9224-D7F283A5EDF4}">
   <dimension ref="A1:S247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="110" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="110" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4681,61 +4683,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="45"/>
       <c r="J1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="48"/>
       <c r="J2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="31" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="18">
@@ -4795,12 +4797,12 @@
         <v>28</v>
       </c>
       <c r="O4" s="2"/>
-      <c r="P4" s="33" t="s">
+      <c r="P4" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="34"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="50"/>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="4" t="s">
@@ -4839,12 +4841,12 @@
         <v>8</v>
       </c>
       <c r="O5" s="2"/>
-      <c r="P5" s="35" t="s">
+      <c r="P5" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="36"/>
+      <c r="Q5" s="39"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="40"/>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="4" t="s">
@@ -4883,12 +4885,12 @@
         <v>2</v>
       </c>
       <c r="O6" s="2"/>
-      <c r="P6" s="35" t="s">
+      <c r="P6" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="36"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="40"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="4" t="s">
@@ -4927,12 +4929,12 @@
         <v>9</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="35" t="s">
+      <c r="P7" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="35"/>
-      <c r="S7" s="36"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="40"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="4" t="s">
@@ -4969,16 +4971,16 @@
       <c r="K8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="39" t="s">
+      <c r="N8" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="40"/>
-      <c r="P8" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="36"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="40"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="4" t="s">
@@ -5013,14 +5015,14 @@
         <v>6</v>
       </c>
       <c r="K9" s="3"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="35" t="s">
+      <c r="N9" s="37"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="36"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="39"/>
+      <c r="S9" s="40"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="4" t="s">
@@ -5103,12 +5105,12 @@
         <v>15</v>
       </c>
       <c r="O11" s="2"/>
-      <c r="P11" s="35" t="s">
+      <c r="P11" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="36"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="40"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1">
       <c r="A12" s="4" t="s">
@@ -5147,12 +5149,12 @@
         <v>16</v>
       </c>
       <c r="O12" s="15"/>
-      <c r="P12" s="37" t="s">
+      <c r="P12" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="37"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="38"/>
+      <c r="Q12" s="35"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="36"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="4" t="s">
@@ -5196,7 +5198,7 @@
         <v>73</v>
       </c>
       <c r="C14" s="3">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>22</v>
@@ -5230,7 +5232,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="3">
-        <v>1938</v>
+        <v>1936</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>22</v>
@@ -5491,7 +5493,7 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="K22" s="51" t="s">
+      <c r="K22" s="53" t="s">
         <v>80</v>
       </c>
     </row>
@@ -5527,7 +5529,7 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="K23" s="52"/>
+      <c r="K23" s="54"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="4" t="s">
@@ -5561,25 +5563,25 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="K24" s="52"/>
+      <c r="K24" s="54"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C25" s="27">
         <v>1939</v>
       </c>
-      <c r="D25" s="43" t="s">
+      <c r="D25" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="44" t="s">
+      <c r="E25" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="43" t="s">
+      <c r="F25" s="27" t="s">
         <v>12</v>
       </c>
       <c r="G25" s="3"/>
@@ -5595,27 +5597,27 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="K25" s="53" t="s">
+      <c r="K25" s="51" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="48" t="s">
+      <c r="A26" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="43">
+      <c r="C26" s="27">
         <v>1939</v>
       </c>
-      <c r="D26" s="43" t="s">
+      <c r="D26" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="44" t="s">
+      <c r="E26" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="43" t="s">
+      <c r="F26" s="27" t="s">
         <v>12</v>
       </c>
       <c r="G26" s="3"/>
@@ -5631,25 +5633,25 @@
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="K26" s="53"/>
+      <c r="K26" s="51"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="43">
+      <c r="C27" s="27">
         <v>1939</v>
       </c>
-      <c r="D27" s="43" t="s">
+      <c r="D27" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="44" t="s">
+      <c r="E27" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="43" t="s">
+      <c r="F27" s="27" t="s">
         <v>12</v>
       </c>
       <c r="G27" s="3"/>
@@ -5665,7 +5667,7 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="K27" s="53"/>
+      <c r="K27" s="51"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="4" t="s">
@@ -5699,8 +5701,8 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="K28" s="53" t="s">
-        <v>85</v>
+      <c r="K28" s="51" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -5735,7 +5737,7 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="K29" s="53"/>
+      <c r="K29" s="51"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="4" t="s">
@@ -5769,11 +5771,11 @@
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="K30" s="53"/>
+      <c r="K30" s="51"/>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>52</v>
@@ -5806,7 +5808,7 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>52</v>
@@ -5839,7 +5841,7 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>52</v>
@@ -5872,13 +5874,13 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>38</v>
@@ -5902,19 +5904,19 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="K34" s="53" t="s">
-        <v>90</v>
+      <c r="K34" s="51" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>38</v>
@@ -5938,17 +5940,17 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="K35" s="53"/>
+      <c r="K35" s="51"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>38</v>
@@ -5972,11 +5974,11 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="K36" s="53"/>
+      <c r="K36" s="51"/>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>40</v>
@@ -6006,13 +6008,13 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="K37" s="53" t="s">
-        <v>92</v>
+      <c r="K37" s="51" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>40</v>
@@ -6042,11 +6044,11 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="K38" s="53"/>
+      <c r="K38" s="51"/>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>40</v>
@@ -6076,11 +6078,11 @@
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="K39" s="53"/>
+      <c r="K39" s="51"/>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>55</v>
@@ -6110,11 +6112,11 @@
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="K40" s="53"/>
+      <c r="K40" s="51"/>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>55</v>
@@ -6144,11 +6146,11 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="K41" s="53"/>
+      <c r="K41" s="51"/>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>55</v>
@@ -6178,14 +6180,14 @@
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="K42" s="53"/>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="K42" s="51"/>
+    </row>
+    <row r="43" spans="1:11" ht="15" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C43" s="3">
         <v>1938</v>
@@ -6212,16 +6214,16 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="K43" s="53" t="s">
-        <v>90</v>
+      <c r="K43" s="51" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C44" s="3">
         <v>1938</v>
@@ -6248,14 +6250,14 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="K44" s="53"/>
+      <c r="K44" s="51"/>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C45" s="3">
         <v>1938</v>
@@ -6282,14 +6284,14 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="K45" s="53"/>
+      <c r="K45" s="51"/>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C46" s="3">
         <v>1942</v>
@@ -6316,16 +6318,16 @@
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="K46" s="50" t="s">
-        <v>97</v>
+      <c r="K46" s="52" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C47" s="3">
         <v>1942</v>
@@ -6352,14 +6354,14 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="K47" s="50"/>
+      <c r="K47" s="52"/>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C48" s="3">
         <v>1942</v>
@@ -6386,11 +6388,11 @@
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="K48" s="50"/>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="K48" s="52"/>
+    </row>
+    <row r="49" spans="1:13" ht="15" customHeight="1">
       <c r="A49" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>52</v>
@@ -6420,13 +6422,13 @@
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="K49" s="53" t="s">
-        <v>90</v>
+      <c r="K49" s="51" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>52</v>
@@ -6456,11 +6458,11 @@
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="K50" s="53"/>
+      <c r="K50" s="51"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>52</v>
@@ -6490,9 +6492,9 @@
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="K51" s="53"/>
+      <c r="K51" s="51"/>
       <c r="M51" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -6515,7 +6517,7 @@
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="K52" s="54"/>
+      <c r="K52" s="34"/>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="4"/>
@@ -7873,7 +7875,7 @@
         <f t="shared" si="6"/>
         <v>Hand_IMU_60_114.txt</v>
       </c>
-      <c r="I117" s="49" t="str">
+      <c r="I117" s="33" t="str">
         <f t="shared" si="7"/>
         <v>Wrist_IMU_60_114.txt</v>
       </c>
@@ -9648,26 +9650,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="P11:S11"/>
+    <mergeCell ref="P12:S12"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="N8:O9"/>
+    <mergeCell ref="K22:K24"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="K37:K39"/>
+    <mergeCell ref="A1:I2"/>
     <mergeCell ref="K40:K42"/>
     <mergeCell ref="K43:K45"/>
     <mergeCell ref="K49:K51"/>
     <mergeCell ref="K46:K48"/>
     <mergeCell ref="K25:K27"/>
-    <mergeCell ref="K22:K24"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="K34:K36"/>
-    <mergeCell ref="K37:K39"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="P11:S11"/>
-    <mergeCell ref="P12:S12"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="N8:O9"/>
-    <mergeCell ref="P7:S7"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="P5:S5"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="P10:S10"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
PCA automation + adding 40s data (35 sets)
</commit_message>
<xml_diff>
--- a/smartglove_data_form.xlsx
+++ b/smartglove_data_form.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kanghae Choi\Dropbox\3_program_code\GITHUB\imaginexlab_smartglove\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BB0B46-9BC5-48A8-88D8-2862AE588B0A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4EF621-2982-48CA-AB80-55D183E48F5E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="478" activeTab="1" xr2:uid="{DEA0BA13-803F-4C08-A035-B07F2889F4B2}"/>
+    <workbookView xWindow="-10785" yWindow="945" windowWidth="21600" windowHeight="11505" tabRatio="478" activeTab="1" xr2:uid="{DEA0BA13-803F-4C08-A035-B07F2889F4B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Data 20s" sheetId="1" r:id="rId1"/>
-    <sheet name="Data 60s" sheetId="2" r:id="rId2"/>
+    <sheet name="Data 40s" sheetId="3" r:id="rId2"/>
+    <sheet name="Data 60s" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -340,6 +341,9 @@
   </si>
   <si>
     <t>Numbed and swollen</t>
+  </si>
+  <si>
+    <t>Manovivo new data 40'</t>
   </si>
 </sst>
 </file>
@@ -816,30 +820,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -864,17 +844,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1195,7 +1199,7 @@
   <dimension ref="A1:S117"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="L65" sqref="L65"/>
+      <selection activeCell="A43" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1214,17 +1218,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="45"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="37"/>
       <c r="J1" t="s">
         <v>17</v>
       </c>
@@ -1233,15 +1237,15 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="48"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="40"/>
       <c r="J2" t="s">
         <v>18</v>
       </c>
@@ -1331,12 +1335,12 @@
         <v>28</v>
       </c>
       <c r="O4" s="2"/>
-      <c r="P4" s="49" t="s">
+      <c r="P4" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="49"/>
-      <c r="S4" s="50"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="42"/>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="4" t="s">
@@ -1377,12 +1381,12 @@
         <v>8</v>
       </c>
       <c r="O5" s="2"/>
-      <c r="P5" s="39" t="s">
+      <c r="P5" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="40"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="44"/>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="4" t="s">
@@ -1423,12 +1427,12 @@
         <v>2</v>
       </c>
       <c r="O6" s="2"/>
-      <c r="P6" s="39" t="s">
+      <c r="P6" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="40"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="44"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="4" t="s">
@@ -1469,12 +1473,12 @@
         <v>9</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="39" t="s">
+      <c r="P7" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="40"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="44"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="4" t="s">
@@ -1511,16 +1515,16 @@
         <v>5</v>
       </c>
       <c r="K8" s="3"/>
-      <c r="N8" s="37" t="s">
+      <c r="N8" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="38"/>
-      <c r="P8" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="40"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="44"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="4" t="s">
@@ -1557,14 +1561,14 @@
         <v>6</v>
       </c>
       <c r="K9" s="3"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="39" t="s">
+      <c r="N9" s="47"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="40"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="44"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="4" t="s">
@@ -1605,12 +1609,12 @@
         <v>14</v>
       </c>
       <c r="O10" s="2"/>
-      <c r="P10" s="41">
+      <c r="P10" s="49">
         <v>4.5891203703703705E-2</v>
       </c>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="41"/>
-      <c r="S10" s="42"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="50"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="4" t="s">
@@ -1651,12 +1655,12 @@
         <v>15</v>
       </c>
       <c r="O11" s="2"/>
-      <c r="P11" s="39" t="s">
+      <c r="P11" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="40"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="44"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1">
       <c r="A12" s="4" t="s">
@@ -1697,12 +1701,12 @@
         <v>16</v>
       </c>
       <c r="O12" s="15"/>
-      <c r="P12" s="35" t="s">
+      <c r="P12" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="36"/>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="46"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="4" t="s">
@@ -4641,17 +4645,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="P5:S5"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="P7:S7"/>
     <mergeCell ref="P12:S12"/>
     <mergeCell ref="N8:O9"/>
     <mergeCell ref="P8:S8"/>
     <mergeCell ref="P9:S9"/>
     <mergeCell ref="P10:S10"/>
     <mergeCell ref="P11:S11"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="P7:S7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4660,10 +4664,3077 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03CA1EFC-6500-4A5D-BEEB-BD0A59C00CDA}">
+  <dimension ref="A1:S117"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="37"/>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="40"/>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A3" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="18">
+        <v>0</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="13"/>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="21" t="str">
+        <f>CONCATENATE("Hand_IMU_40_",J3+1,".txt")</f>
+        <v>Hand_IMU_40_1.txt</v>
+      </c>
+      <c r="I4" s="22" t="str">
+        <f>CONCATENATE("Wrist_IMU_40_",J3+1,".txt")</f>
+        <v>Wrist_IMU_40_1.txt</v>
+      </c>
+      <c r="J4" s="10">
+        <f>J3+1</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="N4" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="42"/>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="3" t="str">
+        <f>CONCATENATE("Hand_IMU_40_",J4+1,".txt")</f>
+        <v>Hand_IMU_40_2.txt</v>
+      </c>
+      <c r="I5" s="5" t="str">
+        <f>CONCATENATE("Wrist_IMU_40_",J4+1,".txt")</f>
+        <v>Wrist_IMU_40_2.txt</v>
+      </c>
+      <c r="J5" s="10">
+        <f t="shared" ref="J5:J68" si="0">J4+1</f>
+        <v>2</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="N5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="44"/>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="21" t="str">
+        <f t="shared" ref="H6:H69" si="1">CONCATENATE("Hand_IMU_40_",J5+1,".txt")</f>
+        <v>Hand_IMU_40_3.txt</v>
+      </c>
+      <c r="I6" s="22" t="str">
+        <f t="shared" ref="I6:I69" si="2">CONCATENATE("Wrist_IMU_40_",J5+1,".txt")</f>
+        <v>Wrist_IMU_40_3.txt</v>
+      </c>
+      <c r="J6" s="10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="N6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="44"/>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_4.txt</v>
+      </c>
+      <c r="I7" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_4.txt</v>
+      </c>
+      <c r="J7" s="10">
+        <f>J6+1</f>
+        <v>4</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="N7" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="44"/>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_5.txt</v>
+      </c>
+      <c r="I8" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_5.txt</v>
+      </c>
+      <c r="J8" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="N8" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" s="48"/>
+      <c r="P8" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="44"/>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_6.txt</v>
+      </c>
+      <c r="I9" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_6.txt</v>
+      </c>
+      <c r="J9" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="44"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_7.txt</v>
+      </c>
+      <c r="I10" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_7.txt</v>
+      </c>
+      <c r="J10" s="10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="N10" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="2"/>
+      <c r="P10" s="49">
+        <v>4.5891203703703705E-2</v>
+      </c>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="50"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_8.txt</v>
+      </c>
+      <c r="I11" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_8.txt</v>
+      </c>
+      <c r="J11" s="10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="N11" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" s="2"/>
+      <c r="P11" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="44"/>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_9.txt</v>
+      </c>
+      <c r="I12" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_9.txt</v>
+      </c>
+      <c r="J12" s="10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K12" s="3"/>
+      <c r="N12" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" s="15"/>
+      <c r="P12" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="46"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_10.txt</v>
+      </c>
+      <c r="I13" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_10.txt</v>
+      </c>
+      <c r="J13" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_11.txt</v>
+      </c>
+      <c r="I14" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_11.txt</v>
+      </c>
+      <c r="J14" s="10">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_12.txt</v>
+      </c>
+      <c r="I15" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_12.txt</v>
+      </c>
+      <c r="J15" s="10">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_13.txt</v>
+      </c>
+      <c r="I16" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_13.txt</v>
+      </c>
+      <c r="J16" s="10">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="M16" t="s">
+        <v>59</v>
+      </c>
+      <c r="O16">
+        <f>SUMPRODUCT(LEN(D4:D63)-LEN(SUBSTITUTE(D4:D63,"M","")))</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_14.txt</v>
+      </c>
+      <c r="I17" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_14.txt</v>
+      </c>
+      <c r="J17" s="10">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="M17" t="s">
+        <v>60</v>
+      </c>
+      <c r="O17">
+        <f>SUMPRODUCT(LEN(D4:D63)-LEN(SUBSTITUTE(D4:D63,"F","")))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_15.txt</v>
+      </c>
+      <c r="I18" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_15.txt</v>
+      </c>
+      <c r="J18" s="10">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="M18" t="s">
+        <v>61</v>
+      </c>
+      <c r="O18">
+        <f>O17/O16</f>
+        <v>1.0588235294117647</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_16.txt</v>
+      </c>
+      <c r="I19" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_16.txt</v>
+      </c>
+      <c r="J19" s="10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_17.txt</v>
+      </c>
+      <c r="I20" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_17.txt</v>
+      </c>
+      <c r="J20" s="10">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="4"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_18.txt</v>
+      </c>
+      <c r="I21" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_18.txt</v>
+      </c>
+      <c r="J21" s="10">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="4"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_19.txt</v>
+      </c>
+      <c r="I22" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_19.txt</v>
+      </c>
+      <c r="J22" s="10">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="4"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_20.txt</v>
+      </c>
+      <c r="I23" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_20.txt</v>
+      </c>
+      <c r="J23" s="10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_21.txt</v>
+      </c>
+      <c r="I24" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_21.txt</v>
+      </c>
+      <c r="J24" s="10">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_22.txt</v>
+      </c>
+      <c r="I25" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_22.txt</v>
+      </c>
+      <c r="J25" s="10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="4"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_23.txt</v>
+      </c>
+      <c r="I26" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_23.txt</v>
+      </c>
+      <c r="J26" s="10">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_24.txt</v>
+      </c>
+      <c r="I27" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_24.txt</v>
+      </c>
+      <c r="J27" s="10">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_25.txt</v>
+      </c>
+      <c r="I28" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_25.txt</v>
+      </c>
+      <c r="J28" s="10">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_26.txt</v>
+      </c>
+      <c r="I29" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_26.txt</v>
+      </c>
+      <c r="J29" s="10">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="4"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_27.txt</v>
+      </c>
+      <c r="I30" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_27.txt</v>
+      </c>
+      <c r="J30" s="10">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="4"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_28.txt</v>
+      </c>
+      <c r="I31" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_28.txt</v>
+      </c>
+      <c r="J31" s="10">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="4"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_29.txt</v>
+      </c>
+      <c r="I32" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_29.txt</v>
+      </c>
+      <c r="J32" s="10">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_30.txt</v>
+      </c>
+      <c r="I33" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_30.txt</v>
+      </c>
+      <c r="J33" s="10">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="4"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_31.txt</v>
+      </c>
+      <c r="I34" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_31.txt</v>
+      </c>
+      <c r="J34" s="10">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="4"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_32.txt</v>
+      </c>
+      <c r="I35" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_32.txt</v>
+      </c>
+      <c r="J35" s="10">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="4"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_33.txt</v>
+      </c>
+      <c r="I36" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_33.txt</v>
+      </c>
+      <c r="J36" s="10">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="4"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_34.txt</v>
+      </c>
+      <c r="I37" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_34.txt</v>
+      </c>
+      <c r="J37" s="10">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="4"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_35.txt</v>
+      </c>
+      <c r="I38" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_35.txt</v>
+      </c>
+      <c r="J38" s="10">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="4"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_36.txt</v>
+      </c>
+      <c r="I39" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_36.txt</v>
+      </c>
+      <c r="J39" s="10">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="4"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H40" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_37.txt</v>
+      </c>
+      <c r="I40" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_37.txt</v>
+      </c>
+      <c r="J40" s="10">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="4"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H41" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_38.txt</v>
+      </c>
+      <c r="I41" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_38.txt</v>
+      </c>
+      <c r="J41" s="10">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="4"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_39.txt</v>
+      </c>
+      <c r="I42" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_39.txt</v>
+      </c>
+      <c r="J42" s="10">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="K42" s="3"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="4"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H43" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_40.txt</v>
+      </c>
+      <c r="I43" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_40.txt</v>
+      </c>
+      <c r="J43" s="10">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="4"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_41.txt</v>
+      </c>
+      <c r="I44" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_41.txt</v>
+      </c>
+      <c r="J44" s="10">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="4"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H45" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_42.txt</v>
+      </c>
+      <c r="I45" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_42.txt</v>
+      </c>
+      <c r="J45" s="10">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="4"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H46" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_43.txt</v>
+      </c>
+      <c r="I46" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_43.txt</v>
+      </c>
+      <c r="J46" s="10">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="4"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H47" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_44.txt</v>
+      </c>
+      <c r="I47" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_44.txt</v>
+      </c>
+      <c r="J47" s="10">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="4"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H48" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_45.txt</v>
+      </c>
+      <c r="I48" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_45.txt</v>
+      </c>
+      <c r="J48" s="10">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="4"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H49" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_46.txt</v>
+      </c>
+      <c r="I49" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_46.txt</v>
+      </c>
+      <c r="J49" s="10">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="K49" s="3"/>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="4"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H50" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_47.txt</v>
+      </c>
+      <c r="I50" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_47.txt</v>
+      </c>
+      <c r="J50" s="10">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="K50" s="3"/>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="4"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H51" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_48.txt</v>
+      </c>
+      <c r="I51" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_48.txt</v>
+      </c>
+      <c r="J51" s="10">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="4"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H52" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_49.txt</v>
+      </c>
+      <c r="I52" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_49.txt</v>
+      </c>
+      <c r="J52" s="10">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="4"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H53" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_50.txt</v>
+      </c>
+      <c r="I53" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_50.txt</v>
+      </c>
+      <c r="J53" s="10">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="K53" s="3"/>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="4"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H54" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_51.txt</v>
+      </c>
+      <c r="I54" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_51.txt</v>
+      </c>
+      <c r="J54" s="10">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="K54" s="3"/>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="4"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H55" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_52.txt</v>
+      </c>
+      <c r="I55" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_52.txt</v>
+      </c>
+      <c r="J55" s="10">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="K55" s="26"/>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="4"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H56" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_53.txt</v>
+      </c>
+      <c r="I56" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_53.txt</v>
+      </c>
+      <c r="J56" s="10">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="K56" s="26"/>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="4"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H57" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_54.txt</v>
+      </c>
+      <c r="I57" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_54.txt</v>
+      </c>
+      <c r="J57" s="10">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="K57" s="26"/>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="4"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H58" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_55.txt</v>
+      </c>
+      <c r="I58" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_55.txt</v>
+      </c>
+      <c r="J58" s="10">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="K58" s="26"/>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="4"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H59" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_56.txt</v>
+      </c>
+      <c r="I59" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_56.txt</v>
+      </c>
+      <c r="J59" s="10">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="K59" s="3"/>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="4"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H60" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_57.txt</v>
+      </c>
+      <c r="I60" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_57.txt</v>
+      </c>
+      <c r="J60" s="10">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="K60" s="3"/>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="4"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H61" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_58.txt</v>
+      </c>
+      <c r="I61" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_58.txt</v>
+      </c>
+      <c r="J61" s="10">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="K61" s="3"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="4"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H62" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_59.txt</v>
+      </c>
+      <c r="I62" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_59.txt</v>
+      </c>
+      <c r="J62" s="10">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="K62" s="3"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="4"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H63" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_60.txt</v>
+      </c>
+      <c r="I63" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_60.txt</v>
+      </c>
+      <c r="J63" s="10">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="K63" s="3"/>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="4"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H64" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_61.txt</v>
+      </c>
+      <c r="I64" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_61.txt</v>
+      </c>
+      <c r="J64" s="10">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="K64" s="3"/>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="4"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H65" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_62.txt</v>
+      </c>
+      <c r="I65" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_62.txt</v>
+      </c>
+      <c r="J65" s="10">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="K65" s="3"/>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" s="4"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H66" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_63.txt</v>
+      </c>
+      <c r="I66" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_63.txt</v>
+      </c>
+      <c r="J66" s="10">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="K66" s="3"/>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" s="4"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H67" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_64.txt</v>
+      </c>
+      <c r="I67" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_64.txt</v>
+      </c>
+      <c r="J67" s="10">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="K67" s="3"/>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" s="4"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H68" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_65.txt</v>
+      </c>
+      <c r="I68" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_65.txt</v>
+      </c>
+      <c r="J68" s="10">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="K68" s="3"/>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="4"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H69" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Hand_IMU_40_66.txt</v>
+      </c>
+      <c r="I69" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Wrist_IMU_40_66.txt</v>
+      </c>
+      <c r="J69" s="10">
+        <f t="shared" ref="J69:J117" si="3">J68+1</f>
+        <v>66</v>
+      </c>
+      <c r="K69" s="3"/>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="4"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H70" s="21" t="str">
+        <f t="shared" ref="H70:H103" si="4">CONCATENATE("Hand_IMU_40_",J69+1,".txt")</f>
+        <v>Hand_IMU_40_67.txt</v>
+      </c>
+      <c r="I70" s="22" t="str">
+        <f t="shared" ref="I70:I103" si="5">CONCATENATE("Wrist_IMU_40_",J69+1,".txt")</f>
+        <v>Wrist_IMU_40_67.txt</v>
+      </c>
+      <c r="J70" s="10">
+        <f t="shared" si="3"/>
+        <v>67</v>
+      </c>
+      <c r="K70" s="3"/>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="4"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H71" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_68.txt</v>
+      </c>
+      <c r="I71" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_68.txt</v>
+      </c>
+      <c r="J71" s="10">
+        <f t="shared" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="K71" s="3"/>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" s="4"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H72" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_69.txt</v>
+      </c>
+      <c r="I72" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_69.txt</v>
+      </c>
+      <c r="J72" s="10">
+        <f t="shared" si="3"/>
+        <v>69</v>
+      </c>
+      <c r="K72" s="3"/>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" s="4"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H73" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_70.txt</v>
+      </c>
+      <c r="I73" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_70.txt</v>
+      </c>
+      <c r="J73" s="10">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="K73" s="3"/>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74" s="4"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H74" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_71.txt</v>
+      </c>
+      <c r="I74" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_71.txt</v>
+      </c>
+      <c r="J74" s="10">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+      <c r="K74" s="3"/>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" s="4"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H75" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_72.txt</v>
+      </c>
+      <c r="I75" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_72.txt</v>
+      </c>
+      <c r="J75" s="10">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="K75" s="3"/>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="4"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H76" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_73.txt</v>
+      </c>
+      <c r="I76" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_73.txt</v>
+      </c>
+      <c r="J76" s="10">
+        <f t="shared" si="3"/>
+        <v>73</v>
+      </c>
+      <c r="K76" s="3"/>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77" s="4"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H77" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_74.txt</v>
+      </c>
+      <c r="I77" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_74.txt</v>
+      </c>
+      <c r="J77" s="10">
+        <f t="shared" si="3"/>
+        <v>74</v>
+      </c>
+      <c r="K77" s="3"/>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" s="4"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H78" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_75.txt</v>
+      </c>
+      <c r="I78" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_75.txt</v>
+      </c>
+      <c r="J78" s="10">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="K78" s="3"/>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" s="4"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H79" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_76.txt</v>
+      </c>
+      <c r="I79" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_76.txt</v>
+      </c>
+      <c r="J79" s="10">
+        <f t="shared" si="3"/>
+        <v>76</v>
+      </c>
+      <c r="K79" s="3"/>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" s="4"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H80" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_77.txt</v>
+      </c>
+      <c r="I80" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_77.txt</v>
+      </c>
+      <c r="J80" s="10">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+      <c r="K80" s="3"/>
+    </row>
+    <row r="81" spans="1:11">
+      <c r="A81" s="4"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H81" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_78.txt</v>
+      </c>
+      <c r="I81" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_78.txt</v>
+      </c>
+      <c r="J81" s="10">
+        <f t="shared" si="3"/>
+        <v>78</v>
+      </c>
+      <c r="K81" s="3"/>
+    </row>
+    <row r="82" spans="1:11">
+      <c r="A82" s="4"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H82" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_79.txt</v>
+      </c>
+      <c r="I82" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_79.txt</v>
+      </c>
+      <c r="J82" s="10">
+        <f t="shared" si="3"/>
+        <v>79</v>
+      </c>
+      <c r="K82" s="3"/>
+    </row>
+    <row r="83" spans="1:11">
+      <c r="A83" s="4"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H83" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_80.txt</v>
+      </c>
+      <c r="I83" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_80.txt</v>
+      </c>
+      <c r="J83" s="10">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="K83" s="3"/>
+    </row>
+    <row r="84" spans="1:11">
+      <c r="A84" s="4"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H84" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_81.txt</v>
+      </c>
+      <c r="I84" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_81.txt</v>
+      </c>
+      <c r="J84" s="10">
+        <f t="shared" si="3"/>
+        <v>81</v>
+      </c>
+      <c r="K84" s="3"/>
+    </row>
+    <row r="85" spans="1:11">
+      <c r="A85" s="4"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H85" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_82.txt</v>
+      </c>
+      <c r="I85" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_82.txt</v>
+      </c>
+      <c r="J85" s="10">
+        <f t="shared" si="3"/>
+        <v>82</v>
+      </c>
+      <c r="K85" s="3"/>
+    </row>
+    <row r="86" spans="1:11">
+      <c r="A86" s="4"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H86" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_83.txt</v>
+      </c>
+      <c r="I86" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_83.txt</v>
+      </c>
+      <c r="J86" s="10">
+        <f t="shared" si="3"/>
+        <v>83</v>
+      </c>
+      <c r="K86" s="3"/>
+    </row>
+    <row r="87" spans="1:11">
+      <c r="A87" s="4"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H87" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_84.txt</v>
+      </c>
+      <c r="I87" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_84.txt</v>
+      </c>
+      <c r="J87" s="10">
+        <f t="shared" si="3"/>
+        <v>84</v>
+      </c>
+      <c r="K87" s="3"/>
+    </row>
+    <row r="88" spans="1:11">
+      <c r="A88" s="4"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H88" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_85.txt</v>
+      </c>
+      <c r="I88" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_85.txt</v>
+      </c>
+      <c r="J88" s="10">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
+      <c r="K88" s="3"/>
+    </row>
+    <row r="89" spans="1:11">
+      <c r="A89" s="4"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H89" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_86.txt</v>
+      </c>
+      <c r="I89" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_86.txt</v>
+      </c>
+      <c r="J89" s="10">
+        <f t="shared" si="3"/>
+        <v>86</v>
+      </c>
+      <c r="K89" s="3"/>
+    </row>
+    <row r="90" spans="1:11">
+      <c r="A90" s="4"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H90" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_87.txt</v>
+      </c>
+      <c r="I90" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_87.txt</v>
+      </c>
+      <c r="J90" s="10">
+        <f t="shared" si="3"/>
+        <v>87</v>
+      </c>
+      <c r="K90" s="3"/>
+    </row>
+    <row r="91" spans="1:11">
+      <c r="A91" s="4"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H91" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_88.txt</v>
+      </c>
+      <c r="I91" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_88.txt</v>
+      </c>
+      <c r="J91" s="10">
+        <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
+      <c r="K91" s="3"/>
+    </row>
+    <row r="92" spans="1:11">
+      <c r="A92" s="4"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H92" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_89.txt</v>
+      </c>
+      <c r="I92" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_89.txt</v>
+      </c>
+      <c r="J92" s="10">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="K92" s="3"/>
+    </row>
+    <row r="93" spans="1:11">
+      <c r="A93" s="4"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H93" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_90.txt</v>
+      </c>
+      <c r="I93" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_90.txt</v>
+      </c>
+      <c r="J93" s="10">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="K93" s="3"/>
+    </row>
+    <row r="94" spans="1:11">
+      <c r="A94" s="4"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H94" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_91.txt</v>
+      </c>
+      <c r="I94" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_91.txt</v>
+      </c>
+      <c r="J94" s="10">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="K94" s="3"/>
+    </row>
+    <row r="95" spans="1:11">
+      <c r="A95" s="4"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H95" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_92.txt</v>
+      </c>
+      <c r="I95" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_92.txt</v>
+      </c>
+      <c r="J95" s="10">
+        <f t="shared" si="3"/>
+        <v>92</v>
+      </c>
+      <c r="K95" s="3"/>
+    </row>
+    <row r="96" spans="1:11">
+      <c r="A96" s="4"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H96" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_93.txt</v>
+      </c>
+      <c r="I96" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_93.txt</v>
+      </c>
+      <c r="J96" s="10">
+        <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+      <c r="K96" s="3"/>
+    </row>
+    <row r="97" spans="1:11">
+      <c r="A97" s="4"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H97" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_94.txt</v>
+      </c>
+      <c r="I97" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_94.txt</v>
+      </c>
+      <c r="J97" s="10">
+        <f t="shared" si="3"/>
+        <v>94</v>
+      </c>
+      <c r="K97" s="3"/>
+    </row>
+    <row r="98" spans="1:11">
+      <c r="A98" s="4"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H98" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_95.txt</v>
+      </c>
+      <c r="I98" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_95.txt</v>
+      </c>
+      <c r="J98" s="10">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="K98" s="3"/>
+    </row>
+    <row r="99" spans="1:11">
+      <c r="A99" s="4"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H99" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_96.txt</v>
+      </c>
+      <c r="I99" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_96.txt</v>
+      </c>
+      <c r="J99" s="10">
+        <f t="shared" si="3"/>
+        <v>96</v>
+      </c>
+      <c r="K99" s="3"/>
+    </row>
+    <row r="100" spans="1:11">
+      <c r="A100" s="4"/>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H100" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_97.txt</v>
+      </c>
+      <c r="I100" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_97.txt</v>
+      </c>
+      <c r="J100" s="10">
+        <f t="shared" si="3"/>
+        <v>97</v>
+      </c>
+      <c r="K100" s="3"/>
+    </row>
+    <row r="101" spans="1:11">
+      <c r="A101" s="4"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H101" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_98.txt</v>
+      </c>
+      <c r="I101" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_98.txt</v>
+      </c>
+      <c r="J101" s="10">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+      <c r="K101" s="3"/>
+    </row>
+    <row r="102" spans="1:11">
+      <c r="A102" s="4"/>
+      <c r="B102" s="3"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H102" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_99.txt</v>
+      </c>
+      <c r="I102" s="22" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_99.txt</v>
+      </c>
+      <c r="J102" s="10">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+      <c r="K102" s="3"/>
+    </row>
+    <row r="103" spans="1:11">
+      <c r="A103" s="4"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H103" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Hand_IMU_40_100.txt</v>
+      </c>
+      <c r="I103" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Wrist_IMU_40_100.txt</v>
+      </c>
+      <c r="J103" s="10">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="K103" s="3"/>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="J104" s="10">
+        <f t="shared" si="3"/>
+        <v>101</v>
+      </c>
+      <c r="K104" s="3"/>
+    </row>
+    <row r="105" spans="1:11">
+      <c r="J105" s="10">
+        <f t="shared" si="3"/>
+        <v>102</v>
+      </c>
+      <c r="K105" s="3"/>
+    </row>
+    <row r="106" spans="1:11">
+      <c r="J106" s="10">
+        <f t="shared" si="3"/>
+        <v>103</v>
+      </c>
+      <c r="K106" s="3"/>
+    </row>
+    <row r="107" spans="1:11">
+      <c r="J107" s="10">
+        <f t="shared" si="3"/>
+        <v>104</v>
+      </c>
+      <c r="K107" s="3"/>
+    </row>
+    <row r="108" spans="1:11">
+      <c r="J108" s="10">
+        <f t="shared" si="3"/>
+        <v>105</v>
+      </c>
+      <c r="K108" s="3"/>
+    </row>
+    <row r="109" spans="1:11">
+      <c r="J109" s="10">
+        <f t="shared" si="3"/>
+        <v>106</v>
+      </c>
+      <c r="K109" s="3"/>
+    </row>
+    <row r="110" spans="1:11">
+      <c r="J110" s="10">
+        <f t="shared" si="3"/>
+        <v>107</v>
+      </c>
+      <c r="K110" s="3"/>
+    </row>
+    <row r="111" spans="1:11">
+      <c r="J111" s="10">
+        <f t="shared" si="3"/>
+        <v>108</v>
+      </c>
+      <c r="K111" s="3"/>
+    </row>
+    <row r="112" spans="1:11">
+      <c r="J112" s="10">
+        <f t="shared" si="3"/>
+        <v>109</v>
+      </c>
+      <c r="K112" s="3"/>
+    </row>
+    <row r="113" spans="10:11">
+      <c r="J113" s="10">
+        <f t="shared" si="3"/>
+        <v>110</v>
+      </c>
+      <c r="K113" s="3"/>
+    </row>
+    <row r="114" spans="10:11">
+      <c r="J114" s="10">
+        <f t="shared" si="3"/>
+        <v>111</v>
+      </c>
+      <c r="K114" s="3"/>
+    </row>
+    <row r="115" spans="10:11">
+      <c r="J115" s="10">
+        <f t="shared" si="3"/>
+        <v>112</v>
+      </c>
+      <c r="K115" s="3"/>
+    </row>
+    <row r="116" spans="10:11">
+      <c r="J116" s="10">
+        <f t="shared" si="3"/>
+        <v>113</v>
+      </c>
+      <c r="K116" s="3"/>
+    </row>
+    <row r="117" spans="10:11">
+      <c r="J117" s="10">
+        <f t="shared" si="3"/>
+        <v>114</v>
+      </c>
+      <c r="K117" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="P11:S11"/>
+    <mergeCell ref="P12:S12"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="N8:O9"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="P9:S9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E86554-00CB-4203-9224-D7F283A5EDF4}">
   <dimension ref="A1:S247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="110" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="110" workbookViewId="0">
       <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
@@ -4683,31 +7754,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="45"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="37"/>
       <c r="J1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="48"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="40"/>
       <c r="J2" t="s">
         <v>18</v>
       </c>
@@ -4797,12 +7868,12 @@
         <v>28</v>
       </c>
       <c r="O4" s="2"/>
-      <c r="P4" s="49" t="s">
+      <c r="P4" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="49"/>
-      <c r="S4" s="50"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="42"/>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="4" t="s">
@@ -4841,12 +7912,12 @@
         <v>8</v>
       </c>
       <c r="O5" s="2"/>
-      <c r="P5" s="39" t="s">
+      <c r="P5" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="40"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="44"/>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="4" t="s">
@@ -4885,12 +7956,12 @@
         <v>2</v>
       </c>
       <c r="O6" s="2"/>
-      <c r="P6" s="39" t="s">
+      <c r="P6" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="40"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="44"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="4" t="s">
@@ -4929,12 +8000,12 @@
         <v>9</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="39" t="s">
+      <c r="P7" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="40"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="44"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="4" t="s">
@@ -4971,16 +8042,16 @@
       <c r="K8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="37" t="s">
+      <c r="N8" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="38"/>
-      <c r="P8" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="40"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="44"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="4" t="s">
@@ -5015,14 +8086,14 @@
         <v>6</v>
       </c>
       <c r="K9" s="3"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="39" t="s">
+      <c r="N9" s="47"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="40"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="44"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="4" t="s">
@@ -5061,12 +8132,12 @@
         <v>14</v>
       </c>
       <c r="O10" s="2"/>
-      <c r="P10" s="41">
+      <c r="P10" s="49">
         <v>4.5891203703703705E-2</v>
       </c>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="41"/>
-      <c r="S10" s="42"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="50"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="4" t="s">
@@ -5105,12 +8176,12 @@
         <v>15</v>
       </c>
       <c r="O11" s="2"/>
-      <c r="P11" s="39" t="s">
+      <c r="P11" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="40"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="44"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1">
       <c r="A12" s="4" t="s">
@@ -5149,12 +8220,12 @@
         <v>16</v>
       </c>
       <c r="O12" s="15"/>
-      <c r="P12" s="35" t="s">
+      <c r="P12" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="36"/>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="46"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="4" t="s">
@@ -5493,7 +8564,7 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="K22" s="53" t="s">
+      <c r="K22" s="51" t="s">
         <v>80</v>
       </c>
     </row>
@@ -5529,7 +8600,7 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="K23" s="54"/>
+      <c r="K23" s="52"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="4" t="s">
@@ -5563,7 +8634,7 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="K24" s="54"/>
+      <c r="K24" s="52"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="32" t="s">
@@ -5597,7 +8668,7 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="K25" s="51" t="s">
+      <c r="K25" s="53" t="s">
         <v>83</v>
       </c>
     </row>
@@ -5633,7 +8704,7 @@
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="K26" s="51"/>
+      <c r="K26" s="53"/>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="32" t="s">
@@ -5667,7 +8738,7 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="K27" s="51"/>
+      <c r="K27" s="53"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="4" t="s">
@@ -5701,7 +8772,7 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="K28" s="51" t="s">
+      <c r="K28" s="53" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5737,7 +8808,7 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="K29" s="51"/>
+      <c r="K29" s="53"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="4" t="s">
@@ -5771,7 +8842,7 @@
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="K30" s="51"/>
+      <c r="K30" s="53"/>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="4" t="s">
@@ -5904,7 +8975,7 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="K34" s="51" t="s">
+      <c r="K34" s="53" t="s">
         <v>98</v>
       </c>
     </row>
@@ -5940,7 +9011,7 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="K35" s="51"/>
+      <c r="K35" s="53"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="4" t="s">
@@ -5974,7 +9045,7 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="K36" s="51"/>
+      <c r="K36" s="53"/>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="4" t="s">
@@ -6008,7 +9079,7 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="K37" s="51" t="s">
+      <c r="K37" s="53" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6044,7 +9115,7 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="K38" s="51"/>
+      <c r="K38" s="53"/>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="4" t="s">
@@ -6078,7 +9149,7 @@
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="K39" s="51"/>
+      <c r="K39" s="53"/>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="4" t="s">
@@ -6112,7 +9183,7 @@
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="K40" s="51"/>
+      <c r="K40" s="53"/>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="4" t="s">
@@ -6146,7 +9217,7 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="K41" s="51"/>
+      <c r="K41" s="53"/>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="4" t="s">
@@ -6180,7 +9251,7 @@
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="K42" s="51"/>
+      <c r="K42" s="53"/>
     </row>
     <row r="43" spans="1:11" ht="15" customHeight="1">
       <c r="A43" s="4" t="s">
@@ -6214,7 +9285,7 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="K43" s="51" t="s">
+      <c r="K43" s="53" t="s">
         <v>98</v>
       </c>
     </row>
@@ -6250,7 +9321,7 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="K44" s="51"/>
+      <c r="K44" s="53"/>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="4" t="s">
@@ -6284,7 +9355,7 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="K45" s="51"/>
+      <c r="K45" s="53"/>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="4" t="s">
@@ -6318,7 +9389,7 @@
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="K46" s="52" t="s">
+      <c r="K46" s="54" t="s">
         <v>96</v>
       </c>
     </row>
@@ -6354,7 +9425,7 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="K47" s="52"/>
+      <c r="K47" s="54"/>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="4" t="s">
@@ -6388,7 +9459,7 @@
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="K48" s="52"/>
+      <c r="K48" s="54"/>
     </row>
     <row r="49" spans="1:13" ht="15" customHeight="1">
       <c r="A49" s="4" t="s">
@@ -6422,7 +9493,7 @@
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="K49" s="51" t="s">
+      <c r="K49" s="53" t="s">
         <v>98</v>
       </c>
     </row>
@@ -6458,7 +9529,7 @@
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="K50" s="51"/>
+      <c r="K50" s="53"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="4" t="s">
@@ -6492,7 +9563,7 @@
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="K51" s="51"/>
+      <c r="K51" s="53"/>
       <c r="M51" t="s">
         <v>95</v>
       </c>
@@ -9650,26 +12721,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="K40:K42"/>
+    <mergeCell ref="K43:K45"/>
+    <mergeCell ref="K49:K51"/>
+    <mergeCell ref="K46:K48"/>
+    <mergeCell ref="K25:K27"/>
+    <mergeCell ref="K22:K24"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="K37:K39"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="P11:S11"/>
+    <mergeCell ref="P12:S12"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="N8:O9"/>
     <mergeCell ref="P7:S7"/>
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="P5:S5"/>
     <mergeCell ref="P4:S4"/>
     <mergeCell ref="P10:S10"/>
-    <mergeCell ref="P11:S11"/>
-    <mergeCell ref="P12:S12"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="N8:O9"/>
-    <mergeCell ref="K22:K24"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="K34:K36"/>
-    <mergeCell ref="K37:K39"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="K40:K42"/>
-    <mergeCell ref="K43:K45"/>
-    <mergeCell ref="K49:K51"/>
-    <mergeCell ref="K46:K48"/>
-    <mergeCell ref="K25:K27"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>